<commit_message>
Fix: add absolute boiling id
</commit_message>
<xml_diff>
--- a/app/data/tests/mascarpone/boiling.xlsx
+++ b/app/data/tests/mascarpone/boiling.xlsx
@@ -1516,7 +1516,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1713,10 +1713,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -12120,7 +12116,7 @@
         <f aca="false">IF(D100="","",VLOOKUP(D100, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C100" s="49" t="str">
+      <c r="C100" s="37" t="str">
         <f aca="false">IF(D100="","",VLOOKUP(D100, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12169,7 +12165,7 @@
         <f aca="false">IF(D101="","",VLOOKUP(D101, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C101" s="49" t="str">
+      <c r="C101" s="37" t="str">
         <f aca="false">IF(D101="","",VLOOKUP(D101, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12218,7 +12214,7 @@
         <f aca="false">IF(D102="","",VLOOKUP(D102, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C102" s="49" t="str">
+      <c r="C102" s="37" t="str">
         <f aca="false">IF(D102="","",VLOOKUP(D102, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12267,7 +12263,7 @@
         <f aca="false">IF(D103="","",VLOOKUP(D103, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C103" s="49" t="str">
+      <c r="C103" s="37" t="str">
         <f aca="false">IF(D103="","",VLOOKUP(D103, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12316,7 +12312,7 @@
         <f aca="false">IF(D104="","",VLOOKUP(D104, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C104" s="49" t="str">
+      <c r="C104" s="37" t="str">
         <f aca="false">IF(D104="","",VLOOKUP(D104, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12365,7 +12361,7 @@
         <f aca="false">IF(D105="","",VLOOKUP(D105, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C105" s="49" t="str">
+      <c r="C105" s="37" t="str">
         <f aca="false">IF(D105="","",VLOOKUP(D105, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12414,7 +12410,7 @@
         <f aca="false">IF(D106="","",VLOOKUP(D106, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C106" s="49" t="str">
+      <c r="C106" s="37" t="str">
         <f aca="false">IF(D106="","",VLOOKUP(D106, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12463,7 +12459,7 @@
         <f aca="false">IF(D107="","",VLOOKUP(D107, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C107" s="49" t="str">
+      <c r="C107" s="37" t="str">
         <f aca="false">IF(D107="","",VLOOKUP(D107, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12512,7 +12508,7 @@
         <f aca="false">IF(D108="","",VLOOKUP(D108, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C108" s="49" t="str">
+      <c r="C108" s="37" t="str">
         <f aca="false">IF(D108="","",VLOOKUP(D108, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12561,7 +12557,7 @@
         <f aca="false">IF(D109="","",VLOOKUP(D109, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C109" s="49" t="str">
+      <c r="C109" s="37" t="str">
         <f aca="false">IF(D109="","",VLOOKUP(D109, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12610,7 +12606,7 @@
         <f aca="false">IF(D110="","",VLOOKUP(D110, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C110" s="49" t="str">
+      <c r="C110" s="37" t="str">
         <f aca="false">IF(D110="","",VLOOKUP(D110, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12659,7 +12655,7 @@
         <f aca="false">IF(D111="","",VLOOKUP(D111, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C111" s="49" t="str">
+      <c r="C111" s="37" t="str">
         <f aca="false">IF(D111="","",VLOOKUP(D111, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12708,7 +12704,7 @@
         <f aca="false">IF(D112="","",VLOOKUP(D112, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C112" s="49" t="str">
+      <c r="C112" s="37" t="str">
         <f aca="false">IF(D112="","",VLOOKUP(D112, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12757,7 +12753,7 @@
         <f aca="false">IF(D113="","",VLOOKUP(D113, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C113" s="49" t="str">
+      <c r="C113" s="37" t="str">
         <f aca="false">IF(D113="","",VLOOKUP(D113, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12806,7 +12802,7 @@
         <f aca="false">IF(D114="","",VLOOKUP(D114, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C114" s="49" t="str">
+      <c r="C114" s="37" t="str">
         <f aca="false">IF(D114="","",VLOOKUP(D114, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12855,7 +12851,7 @@
         <f aca="false">IF(D115="","",VLOOKUP(D115, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C115" s="49" t="str">
+      <c r="C115" s="37" t="str">
         <f aca="false">IF(D115="","",VLOOKUP(D115, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12900,11 +12896,11 @@
       <c r="AMJ115" s="2"/>
     </row>
     <row r="116" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="49" t="str">
+      <c r="B116" s="37" t="str">
         <f aca="false">IF(D116="","",VLOOKUP(D116, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C116" s="49" t="str">
+      <c r="C116" s="37" t="str">
         <f aca="false">IF(D116="","",VLOOKUP(D116, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12949,11 +12945,11 @@
       <c r="AMJ116" s="2"/>
     </row>
     <row r="117" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="49" t="str">
+      <c r="B117" s="37" t="str">
         <f aca="false">IF(D117="","",VLOOKUP(D117, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C117" s="49" t="str">
+      <c r="C117" s="37" t="str">
         <f aca="false">IF(D117="","",VLOOKUP(D117, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -12998,11 +12994,11 @@
       <c r="AMJ117" s="2"/>
     </row>
     <row r="118" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="49" t="str">
+      <c r="B118" s="37" t="str">
         <f aca="false">IF(D118="","",VLOOKUP(D118, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C118" s="49" t="str">
+      <c r="C118" s="37" t="str">
         <f aca="false">IF(D118="","",VLOOKUP(D118, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -13047,11 +13043,11 @@
       <c r="AMJ118" s="2"/>
     </row>
     <row r="119" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="49" t="str">
+      <c r="B119" s="37" t="str">
         <f aca="false">IF(D119="","",VLOOKUP(D119, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C119" s="49" t="str">
+      <c r="C119" s="37" t="str">
         <f aca="false">IF(D119="","",VLOOKUP(D119, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -13096,11 +13092,11 @@
       <c r="AMJ119" s="2"/>
     </row>
     <row r="120" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="49" t="str">
+      <c r="B120" s="37" t="str">
         <f aca="false">IF(D120="","",VLOOKUP(D120, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C120" s="49" t="str">
+      <c r="C120" s="37" t="str">
         <f aca="false">IF(D120="","",VLOOKUP(D120, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -13145,11 +13141,11 @@
       <c r="AMJ120" s="2"/>
     </row>
     <row r="121" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="49" t="str">
+      <c r="B121" s="37" t="str">
         <f aca="false">IF(D121="","",VLOOKUP(D121, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
-      <c r="C121" s="49" t="str">
+      <c r="C121" s="37" t="str">
         <f aca="false">IF(D121="","",VLOOKUP(D121, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -13194,8 +13190,8 @@
       <c r="AMJ121" s="2"/>
     </row>
     <row r="122" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B122" s="49"/>
-      <c r="C122" s="49"/>
+      <c r="B122" s="37"/>
+      <c r="C122" s="37"/>
       <c r="E122" s="36"/>
       <c r="F122" s="33" t="str">
         <f aca="true">IF(I122="","",(INDIRECT("N" &amp; ROW() - 1) - M122))</f>
@@ -13221,8 +13217,8 @@
       <c r="AMJ122" s="2"/>
     </row>
     <row r="123" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B123" s="49"/>
-      <c r="C123" s="49"/>
+      <c r="B123" s="37"/>
+      <c r="C123" s="37"/>
       <c r="E123" s="36"/>
       <c r="F123" s="33" t="str">
         <f aca="true">IF(I123="","",(INDIRECT("N" &amp; ROW() - 1) - M123))</f>
@@ -13248,8 +13244,8 @@
       <c r="AMJ123" s="2"/>
     </row>
     <row r="124" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B124" s="49"/>
-      <c r="C124" s="49"/>
+      <c r="B124" s="37"/>
+      <c r="C124" s="37"/>
       <c r="E124" s="36"/>
       <c r="F124" s="33" t="str">
         <f aca="true">IF(I124="","",(INDIRECT("N" &amp; ROW() - 1) - M124))</f>
@@ -13275,8 +13271,8 @@
       <c r="AMJ124" s="2"/>
     </row>
     <row r="125" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B125" s="49"/>
-      <c r="C125" s="49"/>
+      <c r="B125" s="37"/>
+      <c r="C125" s="37"/>
       <c r="E125" s="36"/>
       <c r="F125" s="33" t="str">
         <f aca="true">IF(I125="","",(INDIRECT("N" &amp; ROW() - 1) - M125))</f>
@@ -13302,8 +13298,8 @@
       <c r="AMJ125" s="2"/>
     </row>
     <row r="126" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B126" s="49"/>
-      <c r="C126" s="49"/>
+      <c r="B126" s="37"/>
+      <c r="C126" s="37"/>
       <c r="E126" s="36"/>
       <c r="F126" s="33" t="str">
         <f aca="true">IF(I126="","",(INDIRECT("N" &amp; ROW() - 1) - M126))</f>
@@ -13329,8 +13325,8 @@
       <c r="AMJ126" s="2"/>
     </row>
     <row r="127" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B127" s="49"/>
-      <c r="C127" s="49"/>
+      <c r="B127" s="37"/>
+      <c r="C127" s="37"/>
       <c r="E127" s="36"/>
       <c r="F127" s="33" t="str">
         <f aca="true">IF(I127="","",(INDIRECT("N" &amp; ROW() - 1) - M127))</f>
@@ -13356,8 +13352,8 @@
       <c r="AMJ127" s="2"/>
     </row>
     <row r="128" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="49"/>
-      <c r="C128" s="49"/>
+      <c r="B128" s="37"/>
+      <c r="C128" s="37"/>
       <c r="E128" s="36"/>
       <c r="F128" s="33" t="str">
         <f aca="true">IF(I128="","",(INDIRECT("N" &amp; ROW() - 1) - M128))</f>
@@ -13383,8 +13379,8 @@
       <c r="AMJ128" s="2"/>
     </row>
     <row r="129" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="49"/>
-      <c r="C129" s="49"/>
+      <c r="B129" s="37"/>
+      <c r="C129" s="37"/>
       <c r="E129" s="36"/>
       <c r="F129" s="33" t="str">
         <f aca="true">IF(I129="","",(INDIRECT("N" &amp; ROW() - 1) - M129))</f>
@@ -13410,8 +13406,8 @@
       <c r="AMJ129" s="2"/>
     </row>
     <row r="130" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="49"/>
-      <c r="C130" s="49"/>
+      <c r="B130" s="37"/>
+      <c r="C130" s="37"/>
       <c r="E130" s="36"/>
       <c r="F130" s="33" t="str">
         <f aca="true">IF(I130="","",(INDIRECT("N" &amp; ROW() - 1) - M130))</f>
@@ -13437,8 +13433,8 @@
       <c r="AMJ130" s="2"/>
     </row>
     <row r="131" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="49"/>
-      <c r="C131" s="49"/>
+      <c r="B131" s="37"/>
+      <c r="C131" s="37"/>
       <c r="E131" s="36"/>
       <c r="F131" s="33" t="str">
         <f aca="true">IF(I131="","",(INDIRECT("N" &amp; ROW() - 1) - M131))</f>
@@ -13464,8 +13460,8 @@
       <c r="AMJ131" s="2"/>
     </row>
     <row r="132" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B132" s="49"/>
-      <c r="C132" s="49"/>
+      <c r="B132" s="37"/>
+      <c r="C132" s="37"/>
       <c r="E132" s="36"/>
       <c r="F132" s="33" t="str">
         <f aca="true">IF(I132="","",(INDIRECT("N" &amp; ROW() - 1) - M132))</f>
@@ -13491,8 +13487,8 @@
       <c r="AMJ132" s="2"/>
     </row>
     <row r="133" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B133" s="49"/>
-      <c r="C133" s="49"/>
+      <c r="B133" s="37"/>
+      <c r="C133" s="37"/>
       <c r="E133" s="36"/>
       <c r="F133" s="33" t="str">
         <f aca="true">IF(I133="","",(INDIRECT("N" &amp; ROW() - 1) - M133))</f>
@@ -13518,8 +13514,8 @@
       <c r="AMJ133" s="2"/>
     </row>
     <row r="134" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B134" s="49"/>
-      <c r="C134" s="49"/>
+      <c r="B134" s="37"/>
+      <c r="C134" s="37"/>
       <c r="E134" s="36"/>
       <c r="F134" s="33" t="str">
         <f aca="true">IF(I134="","",(INDIRECT("N" &amp; ROW() - 1) - M134))</f>
@@ -13545,8 +13541,8 @@
       <c r="AMJ134" s="2"/>
     </row>
     <row r="135" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B135" s="49"/>
-      <c r="C135" s="49"/>
+      <c r="B135" s="37"/>
+      <c r="C135" s="37"/>
       <c r="E135" s="36"/>
       <c r="F135" s="33" t="str">
         <f aca="true">IF(I135="","",(INDIRECT("N" &amp; ROW() - 1) - M135))</f>
@@ -13572,8 +13568,8 @@
       <c r="AMJ135" s="2"/>
     </row>
     <row r="136" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="49"/>
-      <c r="C136" s="49"/>
+      <c r="B136" s="37"/>
+      <c r="C136" s="37"/>
       <c r="E136" s="36"/>
       <c r="F136" s="33" t="str">
         <f aca="true">IF(I136="","",(INDIRECT("N" &amp; ROW() - 1) - M136))</f>
@@ -13599,8 +13595,8 @@
       <c r="AMJ136" s="2"/>
     </row>
     <row r="137" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="49"/>
-      <c r="C137" s="49"/>
+      <c r="B137" s="37"/>
+      <c r="C137" s="37"/>
       <c r="E137" s="36"/>
       <c r="F137" s="33" t="str">
         <f aca="true">IF(I137="","",(INDIRECT("N" &amp; ROW() - 1) - M137))</f>
@@ -13626,8 +13622,8 @@
       <c r="AMJ137" s="2"/>
     </row>
     <row r="138" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B138" s="49"/>
-      <c r="C138" s="49"/>
+      <c r="B138" s="37"/>
+      <c r="C138" s="37"/>
       <c r="E138" s="36"/>
       <c r="F138" s="33" t="str">
         <f aca="true">IF(I138="","",(INDIRECT("N" &amp; ROW() - 1) - M138))</f>
@@ -13653,8 +13649,8 @@
       <c r="AMJ138" s="2"/>
     </row>
     <row r="139" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B139" s="49"/>
-      <c r="C139" s="49"/>
+      <c r="B139" s="37"/>
+      <c r="C139" s="37"/>
       <c r="E139" s="36"/>
       <c r="F139" s="33" t="str">
         <f aca="true">IF(I139="","",(INDIRECT("N" &amp; ROW() - 1) - M139))</f>
@@ -13680,8 +13676,8 @@
       <c r="AMJ139" s="2"/>
     </row>
     <row r="140" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B140" s="49"/>
-      <c r="C140" s="49"/>
+      <c r="B140" s="37"/>
+      <c r="C140" s="37"/>
       <c r="E140" s="36"/>
       <c r="F140" s="33" t="str">
         <f aca="true">IF(I140="","",(INDIRECT("N" &amp; ROW() - 1) - M140))</f>
@@ -13707,8 +13703,8 @@
       <c r="AMJ140" s="2"/>
     </row>
     <row r="141" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B141" s="49"/>
-      <c r="C141" s="49"/>
+      <c r="B141" s="37"/>
+      <c r="C141" s="37"/>
       <c r="E141" s="36"/>
       <c r="F141" s="33" t="str">
         <f aca="true">IF(I141="","",(INDIRECT("N" &amp; ROW() - 1) - M141))</f>
@@ -13734,8 +13730,8 @@
       <c r="AMJ141" s="2"/>
     </row>
     <row r="142" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="49"/>
-      <c r="C142" s="49"/>
+      <c r="B142" s="37"/>
+      <c r="C142" s="37"/>
       <c r="E142" s="36"/>
       <c r="F142" s="33" t="str">
         <f aca="true">IF(I142="","",(INDIRECT("N" &amp; ROW() - 1) - M142))</f>
@@ -13761,8 +13757,8 @@
       <c r="AMJ142" s="2"/>
     </row>
     <row r="143" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B143" s="49"/>
-      <c r="C143" s="49"/>
+      <c r="B143" s="37"/>
+      <c r="C143" s="37"/>
       <c r="E143" s="36"/>
       <c r="F143" s="33" t="str">
         <f aca="true">IF(I143="","",(INDIRECT("N" &amp; ROW() - 1) - M143))</f>
@@ -13788,8 +13784,8 @@
       <c r="AMJ143" s="2"/>
     </row>
     <row r="144" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B144" s="49"/>
-      <c r="C144" s="49"/>
+      <c r="B144" s="37"/>
+      <c r="C144" s="37"/>
       <c r="E144" s="36"/>
       <c r="F144" s="33" t="str">
         <f aca="true">IF(I144="","",(INDIRECT("N" &amp; ROW() - 1) - M144))</f>
@@ -13815,8 +13811,8 @@
       <c r="AMJ144" s="2"/>
     </row>
     <row r="145" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B145" s="49"/>
-      <c r="C145" s="49"/>
+      <c r="B145" s="37"/>
+      <c r="C145" s="37"/>
       <c r="E145" s="36"/>
       <c r="F145" s="33" t="str">
         <f aca="true">IF(I145="","",(INDIRECT("N" &amp; ROW() - 1) - M145))</f>
@@ -13842,8 +13838,8 @@
       <c r="AMJ145" s="2"/>
     </row>
     <row r="146" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="49"/>
-      <c r="C146" s="49"/>
+      <c r="B146" s="37"/>
+      <c r="C146" s="37"/>
       <c r="E146" s="36"/>
       <c r="F146" s="33" t="str">
         <f aca="true">IF(I146="","",(INDIRECT("N" &amp; ROW() - 1) - M146))</f>
@@ -13869,8 +13865,8 @@
       <c r="AMJ146" s="2"/>
     </row>
     <row r="147" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="49"/>
-      <c r="C147" s="49"/>
+      <c r="B147" s="37"/>
+      <c r="C147" s="37"/>
       <c r="E147" s="36"/>
       <c r="F147" s="33" t="str">
         <f aca="true">IF(I147="","",(INDIRECT("N" &amp; ROW() - 1) - M147))</f>
@@ -13896,8 +13892,8 @@
       <c r="AMJ147" s="2"/>
     </row>
     <row r="148" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B148" s="49"/>
-      <c r="C148" s="49"/>
+      <c r="B148" s="37"/>
+      <c r="C148" s="37"/>
       <c r="E148" s="36"/>
       <c r="F148" s="33" t="str">
         <f aca="true">IF(I148="","",(INDIRECT("N" &amp; ROW() - 1) - M148))</f>
@@ -13923,8 +13919,8 @@
       <c r="AMJ148" s="2"/>
     </row>
     <row r="149" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B149" s="49"/>
-      <c r="C149" s="49"/>
+      <c r="B149" s="37"/>
+      <c r="C149" s="37"/>
       <c r="E149" s="36"/>
       <c r="F149" s="33" t="str">
         <f aca="true">IF(I149="","",(INDIRECT("N" &amp; ROW() - 1) - M149))</f>
@@ -13950,8 +13946,8 @@
       <c r="AMJ149" s="2"/>
     </row>
     <row r="150" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B150" s="49"/>
-      <c r="C150" s="49"/>
+      <c r="B150" s="37"/>
+      <c r="C150" s="37"/>
       <c r="E150" s="36"/>
       <c r="F150" s="33" t="str">
         <f aca="true">IF(I150="","",(INDIRECT("N" &amp; ROW() - 1) - M150))</f>
@@ -13977,8 +13973,8 @@
       <c r="AMJ150" s="2"/>
     </row>
     <row r="151" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B151" s="49"/>
-      <c r="C151" s="49"/>
+      <c r="B151" s="37"/>
+      <c r="C151" s="37"/>
       <c r="E151" s="36"/>
       <c r="F151" s="33" t="str">
         <f aca="true">IF(I151="","",(INDIRECT("N" &amp; ROW() - 1) - M151))</f>
@@ -14004,8 +14000,8 @@
       <c r="AMJ151" s="2"/>
     </row>
     <row r="152" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="49"/>
-      <c r="C152" s="49"/>
+      <c r="B152" s="37"/>
+      <c r="C152" s="37"/>
       <c r="E152" s="36"/>
       <c r="F152" s="33" t="str">
         <f aca="true">IF(I152="","",(INDIRECT("N" &amp; ROW() - 1) - M152))</f>
@@ -14031,8 +14027,8 @@
       <c r="AMJ152" s="2"/>
     </row>
     <row r="153" s="35" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="49"/>
-      <c r="C153" s="49"/>
+      <c r="B153" s="37"/>
+      <c r="C153" s="37"/>
       <c r="E153" s="36"/>
       <c r="F153" s="33" t="str">
         <f aca="true">IF(I153="","",(INDIRECT("N" &amp; ROW() - 1) - M153))</f>
@@ -14058,2327 +14054,2327 @@
       <c r="AMJ153" s="2"/>
     </row>
     <row r="154" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B154" s="49"/>
-      <c r="C154" s="49"/>
-      <c r="E154" s="50"/>
-      <c r="F154" s="51" t="str">
+      <c r="B154" s="37"/>
+      <c r="C154" s="37"/>
+      <c r="E154" s="49"/>
+      <c r="F154" s="50" t="str">
         <f aca="true">IF(I154="","",(INDIRECT("N" &amp; ROW() - 1) - M154))</f>
         <v/>
       </c>
-      <c r="G154" s="52" t="str">
+      <c r="G154" s="51" t="str">
         <f aca="true">IF(I154 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H154" s="52" t="str">
+      <c r="H154" s="51" t="str">
         <f aca="true">IF(I154 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q154" s="53" t="str">
+      <c r="Q154" s="52" t="str">
         <f aca="true">IF(P154 = "", "", P154 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R154" s="53" t="str">
+      <c r="R154" s="52" t="str">
         <f aca="true">IF(I154="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B155" s="49"/>
-      <c r="C155" s="49"/>
-      <c r="E155" s="50"/>
-      <c r="F155" s="51" t="str">
+      <c r="B155" s="37"/>
+      <c r="C155" s="37"/>
+      <c r="E155" s="49"/>
+      <c r="F155" s="50" t="str">
         <f aca="true">IF(I155="","",(INDIRECT("N" &amp; ROW() - 1) - M155))</f>
         <v/>
       </c>
-      <c r="G155" s="52" t="str">
+      <c r="G155" s="51" t="str">
         <f aca="true">IF(I155 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H155" s="52" t="str">
+      <c r="H155" s="51" t="str">
         <f aca="true">IF(I155 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q155" s="53" t="str">
+      <c r="Q155" s="52" t="str">
         <f aca="true">IF(P155 = "", "", P155 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R155" s="53" t="str">
+      <c r="R155" s="52" t="str">
         <f aca="true">IF(I155="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B156" s="49"/>
-      <c r="C156" s="49"/>
-      <c r="E156" s="50"/>
-      <c r="F156" s="51" t="str">
+      <c r="B156" s="37"/>
+      <c r="C156" s="37"/>
+      <c r="E156" s="49"/>
+      <c r="F156" s="50" t="str">
         <f aca="true">IF(I156="","",(INDIRECT("N" &amp; ROW() - 1) - M156))</f>
         <v/>
       </c>
-      <c r="G156" s="52" t="str">
+      <c r="G156" s="51" t="str">
         <f aca="true">IF(I156 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H156" s="52" t="str">
+      <c r="H156" s="51" t="str">
         <f aca="true">IF(I156 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q156" s="53" t="str">
+      <c r="Q156" s="52" t="str">
         <f aca="true">IF(P156 = "", "", P156 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R156" s="53" t="str">
+      <c r="R156" s="52" t="str">
         <f aca="true">IF(I156="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B157" s="49"/>
-      <c r="C157" s="49"/>
-      <c r="E157" s="50"/>
-      <c r="F157" s="51" t="str">
+      <c r="B157" s="37"/>
+      <c r="C157" s="37"/>
+      <c r="E157" s="49"/>
+      <c r="F157" s="50" t="str">
         <f aca="true">IF(I157="","",(INDIRECT("N" &amp; ROW() - 1) - M157))</f>
         <v/>
       </c>
-      <c r="G157" s="52" t="str">
+      <c r="G157" s="51" t="str">
         <f aca="true">IF(I157 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H157" s="52" t="str">
+      <c r="H157" s="51" t="str">
         <f aca="true">IF(I157 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q157" s="53" t="str">
+      <c r="Q157" s="52" t="str">
         <f aca="true">IF(P157 = "", "", P157 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R157" s="53" t="str">
+      <c r="R157" s="52" t="str">
         <f aca="true">IF(I157="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="49"/>
-      <c r="C158" s="49"/>
-      <c r="E158" s="50"/>
-      <c r="F158" s="51" t="str">
+      <c r="B158" s="37"/>
+      <c r="C158" s="37"/>
+      <c r="E158" s="49"/>
+      <c r="F158" s="50" t="str">
         <f aca="true">IF(I158="","",(INDIRECT("N" &amp; ROW() - 1) - M158))</f>
         <v/>
       </c>
-      <c r="G158" s="52" t="str">
+      <c r="G158" s="51" t="str">
         <f aca="true">IF(I158 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H158" s="52" t="str">
+      <c r="H158" s="51" t="str">
         <f aca="true">IF(I158 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q158" s="53" t="str">
+      <c r="Q158" s="52" t="str">
         <f aca="true">IF(P158 = "", "", P158 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R158" s="53" t="str">
+      <c r="R158" s="52" t="str">
         <f aca="true">IF(I158="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="49"/>
-      <c r="C159" s="49"/>
-      <c r="E159" s="50"/>
-      <c r="F159" s="51" t="str">
+      <c r="B159" s="37"/>
+      <c r="C159" s="37"/>
+      <c r="E159" s="49"/>
+      <c r="F159" s="50" t="str">
         <f aca="true">IF(I159="","",(INDIRECT("N" &amp; ROW() - 1) - M159))</f>
         <v/>
       </c>
-      <c r="G159" s="52" t="str">
+      <c r="G159" s="51" t="str">
         <f aca="true">IF(I159 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H159" s="52" t="str">
+      <c r="H159" s="51" t="str">
         <f aca="true">IF(I159 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q159" s="53" t="str">
+      <c r="Q159" s="52" t="str">
         <f aca="true">IF(P159 = "", "", P159 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R159" s="53" t="str">
+      <c r="R159" s="52" t="str">
         <f aca="true">IF(I159="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="49"/>
-      <c r="C160" s="49"/>
-      <c r="E160" s="50"/>
-      <c r="F160" s="51" t="str">
+      <c r="B160" s="37"/>
+      <c r="C160" s="37"/>
+      <c r="E160" s="49"/>
+      <c r="F160" s="50" t="str">
         <f aca="true">IF(I160="","",(INDIRECT("N" &amp; ROW() - 1) - M160))</f>
         <v/>
       </c>
-      <c r="G160" s="52" t="str">
+      <c r="G160" s="51" t="str">
         <f aca="true">IF(I160 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H160" s="52" t="str">
+      <c r="H160" s="51" t="str">
         <f aca="true">IF(I160 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q160" s="53" t="str">
+      <c r="Q160" s="52" t="str">
         <f aca="true">IF(P160 = "", "", P160 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R160" s="53" t="str">
+      <c r="R160" s="52" t="str">
         <f aca="true">IF(I160="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="49"/>
-      <c r="C161" s="49"/>
-      <c r="E161" s="50"/>
-      <c r="F161" s="51" t="str">
+      <c r="B161" s="37"/>
+      <c r="C161" s="37"/>
+      <c r="E161" s="49"/>
+      <c r="F161" s="50" t="str">
         <f aca="true">IF(I161="","",(INDIRECT("N" &amp; ROW() - 1) - M161))</f>
         <v/>
       </c>
-      <c r="G161" s="52" t="str">
+      <c r="G161" s="51" t="str">
         <f aca="true">IF(I161 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H161" s="52" t="str">
+      <c r="H161" s="51" t="str">
         <f aca="true">IF(I161 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q161" s="53" t="str">
+      <c r="Q161" s="52" t="str">
         <f aca="true">IF(P161 = "", "", P161 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R161" s="53" t="str">
+      <c r="R161" s="52" t="str">
         <f aca="true">IF(I161="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="49"/>
-      <c r="C162" s="49"/>
-      <c r="E162" s="50"/>
-      <c r="F162" s="51" t="str">
+      <c r="B162" s="37"/>
+      <c r="C162" s="37"/>
+      <c r="E162" s="49"/>
+      <c r="F162" s="50" t="str">
         <f aca="true">IF(I162="","",(INDIRECT("N" &amp; ROW() - 1) - M162))</f>
         <v/>
       </c>
-      <c r="G162" s="52" t="str">
+      <c r="G162" s="51" t="str">
         <f aca="true">IF(I162 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H162" s="52" t="str">
+      <c r="H162" s="51" t="str">
         <f aca="true">IF(I162 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q162" s="53" t="str">
+      <c r="Q162" s="52" t="str">
         <f aca="true">IF(P162 = "", "", P162 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R162" s="53" t="str">
+      <c r="R162" s="52" t="str">
         <f aca="true">IF(I162="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="49"/>
-      <c r="C163" s="49"/>
-      <c r="E163" s="50"/>
-      <c r="F163" s="51" t="str">
+      <c r="B163" s="37"/>
+      <c r="C163" s="37"/>
+      <c r="E163" s="49"/>
+      <c r="F163" s="50" t="str">
         <f aca="true">IF(I163="","",(INDIRECT("N" &amp; ROW() - 1) - M163))</f>
         <v/>
       </c>
-      <c r="G163" s="52" t="str">
+      <c r="G163" s="51" t="str">
         <f aca="true">IF(I163 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H163" s="52" t="str">
+      <c r="H163" s="51" t="str">
         <f aca="true">IF(I163 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q163" s="53" t="str">
+      <c r="Q163" s="52" t="str">
         <f aca="true">IF(P163 = "", "", P163 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R163" s="53" t="str">
+      <c r="R163" s="52" t="str">
         <f aca="true">IF(I163="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="49"/>
-      <c r="C164" s="49"/>
-      <c r="E164" s="50"/>
-      <c r="F164" s="51" t="str">
+      <c r="B164" s="37"/>
+      <c r="C164" s="37"/>
+      <c r="E164" s="49"/>
+      <c r="F164" s="50" t="str">
         <f aca="true">IF(I164="","",(INDIRECT("N" &amp; ROW() - 1) - M164))</f>
         <v/>
       </c>
-      <c r="H164" s="52" t="str">
+      <c r="H164" s="51" t="str">
         <f aca="true">IF(I164 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q164" s="53" t="str">
+      <c r="Q164" s="52" t="str">
         <f aca="true">IF(P164 = "", "", P164 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R164" s="53" t="str">
+      <c r="R164" s="52" t="str">
         <f aca="true">IF(I164="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="49"/>
-      <c r="C165" s="49"/>
-      <c r="E165" s="50"/>
-      <c r="F165" s="51" t="str">
+      <c r="B165" s="37"/>
+      <c r="C165" s="37"/>
+      <c r="E165" s="49"/>
+      <c r="F165" s="50" t="str">
         <f aca="true">IF(I165="","",(INDIRECT("N" &amp; ROW() - 1) - M165))</f>
         <v/>
       </c>
-      <c r="H165" s="52" t="str">
+      <c r="H165" s="51" t="str">
         <f aca="true">IF(I165 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q165" s="53" t="str">
+      <c r="Q165" s="52" t="str">
         <f aca="true">IF(P165 = "", "", P165 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R165" s="53" t="str">
+      <c r="R165" s="52" t="str">
         <f aca="true">IF(I165="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="49"/>
-      <c r="C166" s="49"/>
-      <c r="E166" s="50"/>
-      <c r="F166" s="51" t="str">
+      <c r="B166" s="37"/>
+      <c r="C166" s="37"/>
+      <c r="E166" s="49"/>
+      <c r="F166" s="50" t="str">
         <f aca="true">IF(I166="","",(INDIRECT("N" &amp; ROW() - 1) - M166))</f>
         <v/>
       </c>
-      <c r="H166" s="52" t="str">
+      <c r="H166" s="51" t="str">
         <f aca="true">IF(I166 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q166" s="53" t="str">
+      <c r="Q166" s="52" t="str">
         <f aca="true">IF(P166 = "", "", P166 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R166" s="53" t="str">
+      <c r="R166" s="52" t="str">
         <f aca="true">IF(I166="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="49"/>
-      <c r="C167" s="49"/>
-      <c r="E167" s="50"/>
-      <c r="F167" s="51" t="str">
+      <c r="B167" s="37"/>
+      <c r="C167" s="37"/>
+      <c r="E167" s="49"/>
+      <c r="F167" s="50" t="str">
         <f aca="true">IF(I167="","",(INDIRECT("N" &amp; ROW() - 1) - M167))</f>
         <v/>
       </c>
-      <c r="H167" s="52" t="str">
+      <c r="H167" s="51" t="str">
         <f aca="true">IF(I167 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q167" s="53" t="str">
+      <c r="Q167" s="52" t="str">
         <f aca="true">IF(P167 = "", "", P167 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R167" s="53" t="str">
+      <c r="R167" s="52" t="str">
         <f aca="true">IF(I167="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="49"/>
-      <c r="C168" s="49"/>
-      <c r="E168" s="50"/>
-      <c r="F168" s="51" t="str">
+      <c r="B168" s="37"/>
+      <c r="C168" s="37"/>
+      <c r="E168" s="49"/>
+      <c r="F168" s="50" t="str">
         <f aca="true">IF(I168="","",(INDIRECT("N" &amp; ROW() - 1) - M168))</f>
         <v/>
       </c>
-      <c r="H168" s="52" t="str">
+      <c r="H168" s="51" t="str">
         <f aca="true">IF(I168 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q168" s="53" t="str">
+      <c r="Q168" s="52" t="str">
         <f aca="true">IF(P168 = "", "", P168 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R168" s="53" t="str">
+      <c r="R168" s="52" t="str">
         <f aca="true">IF(I168="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="49"/>
-      <c r="C169" s="49"/>
-      <c r="E169" s="50"/>
-      <c r="F169" s="51" t="str">
+      <c r="B169" s="37"/>
+      <c r="C169" s="37"/>
+      <c r="E169" s="49"/>
+      <c r="F169" s="50" t="str">
         <f aca="true">IF(I169="","",(INDIRECT("N" &amp; ROW() - 1) - M169))</f>
         <v/>
       </c>
-      <c r="H169" s="52" t="str">
+      <c r="H169" s="51" t="str">
         <f aca="true">IF(I169 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q169" s="53" t="str">
+      <c r="Q169" s="52" t="str">
         <f aca="true">IF(P169 = "", "", P169 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R169" s="53" t="str">
+      <c r="R169" s="52" t="str">
         <f aca="true">IF(I169="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="49"/>
-      <c r="C170" s="49"/>
-      <c r="E170" s="50"/>
-      <c r="F170" s="51" t="str">
+      <c r="B170" s="37"/>
+      <c r="C170" s="37"/>
+      <c r="E170" s="49"/>
+      <c r="F170" s="50" t="str">
         <f aca="true">IF(I170="","",(INDIRECT("N" &amp; ROW() - 1) - M170))</f>
         <v/>
       </c>
-      <c r="H170" s="52" t="str">
+      <c r="H170" s="51" t="str">
         <f aca="true">IF(I170 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q170" s="53" t="str">
+      <c r="Q170" s="52" t="str">
         <f aca="true">IF(P170 = "", "", P170 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R170" s="53" t="str">
+      <c r="R170" s="52" t="str">
         <f aca="true">IF(I170="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="49"/>
-      <c r="C171" s="49"/>
-      <c r="E171" s="50"/>
-      <c r="F171" s="51" t="str">
+      <c r="B171" s="37"/>
+      <c r="C171" s="37"/>
+      <c r="E171" s="49"/>
+      <c r="F171" s="50" t="str">
         <f aca="true">IF(I171="","",(INDIRECT("N" &amp; ROW() - 1) - M171))</f>
         <v/>
       </c>
-      <c r="H171" s="52" t="str">
+      <c r="H171" s="51" t="str">
         <f aca="true">IF(I171 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q171" s="53" t="str">
+      <c r="Q171" s="52" t="str">
         <f aca="true">IF(P171 = "", "", P171 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R171" s="53" t="str">
+      <c r="R171" s="52" t="str">
         <f aca="true">IF(I171="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="49"/>
-      <c r="C172" s="49"/>
-      <c r="E172" s="50"/>
-      <c r="F172" s="51" t="str">
+      <c r="B172" s="37"/>
+      <c r="C172" s="37"/>
+      <c r="E172" s="49"/>
+      <c r="F172" s="50" t="str">
         <f aca="true">IF(I172="","",(INDIRECT("N" &amp; ROW() - 1) - M172))</f>
         <v/>
       </c>
-      <c r="H172" s="52" t="str">
+      <c r="H172" s="51" t="str">
         <f aca="true">IF(I172 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q172" s="53" t="str">
+      <c r="Q172" s="52" t="str">
         <f aca="true">IF(P172 = "", "", P172 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R172" s="53" t="str">
+      <c r="R172" s="52" t="str">
         <f aca="true">IF(I172="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B173" s="49"/>
-      <c r="C173" s="49"/>
-      <c r="E173" s="50"/>
-      <c r="F173" s="51" t="str">
+      <c r="B173" s="37"/>
+      <c r="C173" s="37"/>
+      <c r="E173" s="49"/>
+      <c r="F173" s="50" t="str">
         <f aca="true">IF(I173="","",(INDIRECT("N" &amp; ROW() - 1) - M173))</f>
         <v/>
       </c>
-      <c r="H173" s="52" t="str">
+      <c r="H173" s="51" t="str">
         <f aca="true">IF(I173 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q173" s="53" t="str">
+      <c r="Q173" s="52" t="str">
         <f aca="true">IF(P173 = "", "", P173 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R173" s="53" t="str">
+      <c r="R173" s="52" t="str">
         <f aca="true">IF(I173="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="49"/>
-      <c r="C174" s="49"/>
-      <c r="E174" s="50"/>
-      <c r="F174" s="51" t="str">
+      <c r="B174" s="37"/>
+      <c r="C174" s="37"/>
+      <c r="E174" s="49"/>
+      <c r="F174" s="50" t="str">
         <f aca="true">IF(I174="","",(INDIRECT("N" &amp; ROW() - 1) - M174))</f>
         <v/>
       </c>
-      <c r="H174" s="52" t="str">
+      <c r="H174" s="51" t="str">
         <f aca="true">IF(I174 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q174" s="53" t="str">
+      <c r="Q174" s="52" t="str">
         <f aca="true">IF(P174 = "", "", P174 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R174" s="53" t="str">
+      <c r="R174" s="52" t="str">
         <f aca="true">IF(I174="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="49"/>
-      <c r="C175" s="49"/>
-      <c r="E175" s="50"/>
-      <c r="F175" s="51" t="str">
+      <c r="B175" s="37"/>
+      <c r="C175" s="37"/>
+      <c r="E175" s="49"/>
+      <c r="F175" s="50" t="str">
         <f aca="true">IF(I175="","",(INDIRECT("N" &amp; ROW() - 1) - M175))</f>
         <v/>
       </c>
-      <c r="H175" s="52" t="str">
+      <c r="H175" s="51" t="str">
         <f aca="true">IF(I175 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q175" s="53" t="str">
+      <c r="Q175" s="52" t="str">
         <f aca="true">IF(P175 = "", "", P175 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R175" s="53" t="str">
+      <c r="R175" s="52" t="str">
         <f aca="true">IF(I175="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="49"/>
-      <c r="C176" s="49"/>
-      <c r="E176" s="50"/>
-      <c r="F176" s="51" t="str">
+      <c r="B176" s="37"/>
+      <c r="C176" s="37"/>
+      <c r="E176" s="49"/>
+      <c r="F176" s="50" t="str">
         <f aca="true">IF(I176="","",(INDIRECT("N" &amp; ROW() - 1) - M176))</f>
         <v/>
       </c>
-      <c r="H176" s="52" t="str">
+      <c r="H176" s="51" t="str">
         <f aca="true">IF(I176 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q176" s="53" t="str">
+      <c r="Q176" s="52" t="str">
         <f aca="true">IF(P176 = "", "", P176 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R176" s="53" t="str">
+      <c r="R176" s="52" t="str">
         <f aca="true">IF(I176="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="49"/>
-      <c r="C177" s="49"/>
-      <c r="E177" s="50"/>
-      <c r="F177" s="51" t="str">
+      <c r="B177" s="37"/>
+      <c r="C177" s="37"/>
+      <c r="E177" s="49"/>
+      <c r="F177" s="50" t="str">
         <f aca="true">IF(I177="","",(INDIRECT("N" &amp; ROW() - 1) - M177))</f>
         <v/>
       </c>
-      <c r="H177" s="52" t="str">
+      <c r="H177" s="51" t="str">
         <f aca="true">IF(I177 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q177" s="53" t="str">
+      <c r="Q177" s="52" t="str">
         <f aca="true">IF(P177 = "", "", P177 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R177" s="53" t="str">
+      <c r="R177" s="52" t="str">
         <f aca="true">IF(I177="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="49"/>
-      <c r="C178" s="49"/>
-      <c r="E178" s="50"/>
-      <c r="F178" s="51" t="str">
+      <c r="B178" s="37"/>
+      <c r="C178" s="37"/>
+      <c r="E178" s="49"/>
+      <c r="F178" s="50" t="str">
         <f aca="true">IF(I178="","",(INDIRECT("N" &amp; ROW() - 1) - M178))</f>
         <v/>
       </c>
-      <c r="H178" s="52" t="str">
+      <c r="H178" s="51" t="str">
         <f aca="true">IF(I178 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q178" s="53" t="str">
+      <c r="Q178" s="52" t="str">
         <f aca="true">IF(P178 = "", "", P178 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R178" s="53" t="str">
+      <c r="R178" s="52" t="str">
         <f aca="true">IF(I178="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="49"/>
-      <c r="C179" s="49"/>
-      <c r="E179" s="50"/>
-      <c r="F179" s="51" t="str">
+      <c r="B179" s="37"/>
+      <c r="C179" s="37"/>
+      <c r="E179" s="49"/>
+      <c r="F179" s="50" t="str">
         <f aca="true">IF(I179="","",(INDIRECT("N" &amp; ROW() - 1) - M179))</f>
         <v/>
       </c>
-      <c r="H179" s="52" t="str">
+      <c r="H179" s="51" t="str">
         <f aca="true">IF(I179 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q179" s="53" t="str">
+      <c r="Q179" s="52" t="str">
         <f aca="true">IF(P179 = "", "", P179 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R179" s="53" t="str">
+      <c r="R179" s="52" t="str">
         <f aca="true">IF(I179="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="49"/>
-      <c r="C180" s="49"/>
-      <c r="E180" s="50"/>
-      <c r="F180" s="51" t="str">
+      <c r="B180" s="37"/>
+      <c r="C180" s="37"/>
+      <c r="E180" s="49"/>
+      <c r="F180" s="50" t="str">
         <f aca="true">IF(I180="","",(INDIRECT("N" &amp; ROW() - 1) - M180))</f>
         <v/>
       </c>
-      <c r="H180" s="52" t="str">
+      <c r="H180" s="51" t="str">
         <f aca="true">IF(I180 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q180" s="53" t="str">
+      <c r="Q180" s="52" t="str">
         <f aca="true">IF(P180 = "", "", P180 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R180" s="53" t="str">
+      <c r="R180" s="52" t="str">
         <f aca="true">IF(I180="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B181" s="49"/>
-      <c r="C181" s="49"/>
-      <c r="E181" s="50"/>
-      <c r="F181" s="51" t="str">
+      <c r="B181" s="37"/>
+      <c r="C181" s="37"/>
+      <c r="E181" s="49"/>
+      <c r="F181" s="50" t="str">
         <f aca="true">IF(I181="","",(INDIRECT("N" &amp; ROW() - 1) - M181))</f>
         <v/>
       </c>
-      <c r="H181" s="52" t="str">
+      <c r="H181" s="51" t="str">
         <f aca="true">IF(I181 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q181" s="53" t="str">
+      <c r="Q181" s="52" t="str">
         <f aca="true">IF(P181 = "", "", P181 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R181" s="53" t="str">
+      <c r="R181" s="52" t="str">
         <f aca="true">IF(I181="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="49"/>
-      <c r="C182" s="49"/>
-      <c r="E182" s="50"/>
-      <c r="F182" s="51" t="str">
+      <c r="B182" s="37"/>
+      <c r="C182" s="37"/>
+      <c r="E182" s="49"/>
+      <c r="F182" s="50" t="str">
         <f aca="true">IF(I182="","",(INDIRECT("N" &amp; ROW() - 1) - M182))</f>
         <v/>
       </c>
-      <c r="H182" s="52" t="str">
+      <c r="H182" s="51" t="str">
         <f aca="true">IF(I182 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q182" s="53" t="str">
+      <c r="Q182" s="52" t="str">
         <f aca="true">IF(P182 = "", "", P182 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R182" s="53" t="str">
+      <c r="R182" s="52" t="str">
         <f aca="true">IF(I182="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="49"/>
-      <c r="C183" s="49"/>
-      <c r="E183" s="50"/>
-      <c r="F183" s="51" t="str">
+      <c r="B183" s="37"/>
+      <c r="C183" s="37"/>
+      <c r="E183" s="49"/>
+      <c r="F183" s="50" t="str">
         <f aca="true">IF(I183="","",(INDIRECT("N" &amp; ROW() - 1) - M183))</f>
         <v/>
       </c>
-      <c r="H183" s="52" t="str">
+      <c r="H183" s="51" t="str">
         <f aca="true">IF(I183 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q183" s="53"/>
-      <c r="R183" s="53" t="str">
+      <c r="Q183" s="52"/>
+      <c r="R183" s="52" t="str">
         <f aca="true">IF(I183="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="49"/>
-      <c r="C184" s="49"/>
-      <c r="E184" s="50"/>
-      <c r="F184" s="51" t="str">
+      <c r="B184" s="37"/>
+      <c r="C184" s="37"/>
+      <c r="E184" s="49"/>
+      <c r="F184" s="50" t="str">
         <f aca="true">IF(I184="","",(INDIRECT("N" &amp; ROW() - 1) - M184))</f>
         <v/>
       </c>
-      <c r="H184" s="52" t="str">
+      <c r="H184" s="51" t="str">
         <f aca="true">IF(I184 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q184" s="53"/>
-      <c r="R184" s="53" t="str">
+      <c r="Q184" s="52"/>
+      <c r="R184" s="52" t="str">
         <f aca="true">IF(I184="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="49"/>
-      <c r="C185" s="49"/>
-      <c r="E185" s="50"/>
-      <c r="F185" s="51" t="str">
+      <c r="B185" s="37"/>
+      <c r="C185" s="37"/>
+      <c r="E185" s="49"/>
+      <c r="F185" s="50" t="str">
         <f aca="true">IF(I185="","",(INDIRECT("N" &amp; ROW() - 1) - M185))</f>
         <v/>
       </c>
-      <c r="H185" s="52" t="str">
+      <c r="H185" s="51" t="str">
         <f aca="true">IF(I185 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q185" s="53"/>
-      <c r="R185" s="53" t="str">
+      <c r="Q185" s="52"/>
+      <c r="R185" s="52" t="str">
         <f aca="true">IF(I185="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="49"/>
-      <c r="C186" s="49"/>
-      <c r="E186" s="50"/>
-      <c r="F186" s="51" t="str">
+      <c r="B186" s="37"/>
+      <c r="C186" s="37"/>
+      <c r="E186" s="49"/>
+      <c r="F186" s="50" t="str">
         <f aca="true">IF(I186="","",(INDIRECT("N" &amp; ROW() - 1) - M186))</f>
         <v/>
       </c>
-      <c r="H186" s="52" t="str">
+      <c r="H186" s="51" t="str">
         <f aca="true">IF(I186 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q186" s="53"/>
-      <c r="R186" s="53" t="str">
+      <c r="Q186" s="52"/>
+      <c r="R186" s="52" t="str">
         <f aca="true">IF(I186="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="49"/>
-      <c r="C187" s="49"/>
-      <c r="E187" s="50"/>
-      <c r="F187" s="51" t="str">
+      <c r="B187" s="37"/>
+      <c r="C187" s="37"/>
+      <c r="E187" s="49"/>
+      <c r="F187" s="50" t="str">
         <f aca="true">IF(I187="","",(INDIRECT("N" &amp; ROW() - 1) - M187))</f>
         <v/>
       </c>
-      <c r="H187" s="52" t="str">
+      <c r="H187" s="51" t="str">
         <f aca="true">IF(I187 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q187" s="53"/>
-      <c r="R187" s="53" t="str">
+      <c r="Q187" s="52"/>
+      <c r="R187" s="52" t="str">
         <f aca="true">IF(I187="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="49"/>
-      <c r="C188" s="49"/>
-      <c r="E188" s="50"/>
-      <c r="F188" s="51" t="str">
+      <c r="B188" s="37"/>
+      <c r="C188" s="37"/>
+      <c r="E188" s="49"/>
+      <c r="F188" s="50" t="str">
         <f aca="true">IF(I188="","",(INDIRECT("N" &amp; ROW() - 1) - M188))</f>
         <v/>
       </c>
-      <c r="H188" s="52" t="str">
+      <c r="H188" s="51" t="str">
         <f aca="true">IF(I188 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q188" s="53"/>
-      <c r="R188" s="53" t="str">
+      <c r="Q188" s="52"/>
+      <c r="R188" s="52" t="str">
         <f aca="true">IF(I188="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B189" s="49"/>
-      <c r="C189" s="49"/>
-      <c r="E189" s="50"/>
-      <c r="F189" s="51" t="str">
+      <c r="B189" s="37"/>
+      <c r="C189" s="37"/>
+      <c r="E189" s="49"/>
+      <c r="F189" s="50" t="str">
         <f aca="true">IF(I189="","",(INDIRECT("N" &amp; ROW() - 1) - M189))</f>
         <v/>
       </c>
-      <c r="H189" s="52" t="str">
+      <c r="H189" s="51" t="str">
         <f aca="true">IF(I189 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q189" s="53"/>
-      <c r="R189" s="53" t="str">
+      <c r="Q189" s="52"/>
+      <c r="R189" s="52" t="str">
         <f aca="true">IF(I189="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="49"/>
-      <c r="C190" s="49"/>
-      <c r="E190" s="50"/>
-      <c r="F190" s="51" t="str">
+      <c r="B190" s="37"/>
+      <c r="C190" s="37"/>
+      <c r="E190" s="49"/>
+      <c r="F190" s="50" t="str">
         <f aca="true">IF(I190="","",(INDIRECT("N" &amp; ROW() - 1) - M190))</f>
         <v/>
       </c>
-      <c r="H190" s="52" t="str">
+      <c r="H190" s="51" t="str">
         <f aca="true">IF(I190 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q190" s="53"/>
-      <c r="R190" s="53" t="str">
+      <c r="Q190" s="52"/>
+      <c r="R190" s="52" t="str">
         <f aca="true">IF(I190="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="49"/>
-      <c r="C191" s="49"/>
-      <c r="E191" s="50"/>
-      <c r="F191" s="51" t="str">
+      <c r="B191" s="37"/>
+      <c r="C191" s="37"/>
+      <c r="E191" s="49"/>
+      <c r="F191" s="50" t="str">
         <f aca="true">IF(I191="","",(INDIRECT("N" &amp; ROW() - 1) - M191))</f>
         <v/>
       </c>
-      <c r="H191" s="52" t="str">
+      <c r="H191" s="51" t="str">
         <f aca="true">IF(I191 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q191" s="53"/>
-      <c r="R191" s="53" t="str">
+      <c r="Q191" s="52"/>
+      <c r="R191" s="52" t="str">
         <f aca="true">IF(I191="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="49"/>
-      <c r="C192" s="49"/>
-      <c r="E192" s="50"/>
-      <c r="F192" s="51" t="str">
+      <c r="B192" s="37"/>
+      <c r="C192" s="37"/>
+      <c r="E192" s="49"/>
+      <c r="F192" s="50" t="str">
         <f aca="true">IF(I192="","",(INDIRECT("N" &amp; ROW() - 1) - M192))</f>
         <v/>
       </c>
-      <c r="H192" s="52" t="str">
+      <c r="H192" s="51" t="str">
         <f aca="true">IF(I192 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q192" s="53"/>
-      <c r="R192" s="53" t="str">
+      <c r="Q192" s="52"/>
+      <c r="R192" s="52" t="str">
         <f aca="true">IF(I192="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="49"/>
-      <c r="C193" s="49"/>
-      <c r="E193" s="50"/>
-      <c r="F193" s="51" t="str">
+      <c r="B193" s="37"/>
+      <c r="C193" s="37"/>
+      <c r="E193" s="49"/>
+      <c r="F193" s="50" t="str">
         <f aca="true">IF(I193="","",(INDIRECT("N" &amp; ROW() - 1) - M193))</f>
         <v/>
       </c>
-      <c r="H193" s="52" t="str">
+      <c r="H193" s="51" t="str">
         <f aca="true">IF(I193 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q193" s="53"/>
-      <c r="R193" s="53" t="str">
+      <c r="Q193" s="52"/>
+      <c r="R193" s="52" t="str">
         <f aca="true">IF(I193="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="49"/>
-      <c r="C194" s="49"/>
-      <c r="E194" s="50"/>
-      <c r="F194" s="51" t="str">
+      <c r="B194" s="37"/>
+      <c r="C194" s="37"/>
+      <c r="E194" s="49"/>
+      <c r="F194" s="50" t="str">
         <f aca="true">IF(I194="","",(INDIRECT("N" &amp; ROW() - 1) - M194))</f>
         <v/>
       </c>
-      <c r="H194" s="52" t="str">
+      <c r="H194" s="51" t="str">
         <f aca="true">IF(I194 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q194" s="53"/>
-      <c r="R194" s="53" t="str">
+      <c r="Q194" s="52"/>
+      <c r="R194" s="52" t="str">
         <f aca="true">IF(I194="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="49"/>
-      <c r="C195" s="49"/>
-      <c r="E195" s="50"/>
-      <c r="F195" s="51" t="str">
+      <c r="B195" s="37"/>
+      <c r="C195" s="37"/>
+      <c r="E195" s="49"/>
+      <c r="F195" s="50" t="str">
         <f aca="true">IF(I195="","",(INDIRECT("N" &amp; ROW() - 1) - M195))</f>
         <v/>
       </c>
-      <c r="H195" s="52" t="str">
+      <c r="H195" s="51" t="str">
         <f aca="true">IF(I195 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q195" s="53"/>
-      <c r="R195" s="53" t="str">
+      <c r="Q195" s="52"/>
+      <c r="R195" s="52" t="str">
         <f aca="true">IF(I195="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="49"/>
-      <c r="C196" s="49"/>
-      <c r="E196" s="50"/>
-      <c r="F196" s="50"/>
-      <c r="H196" s="52" t="str">
+      <c r="B196" s="37"/>
+      <c r="C196" s="37"/>
+      <c r="E196" s="49"/>
+      <c r="F196" s="49"/>
+      <c r="H196" s="51" t="str">
         <f aca="true">IF(I196 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q196" s="53"/>
-      <c r="R196" s="53" t="str">
+      <c r="Q196" s="52"/>
+      <c r="R196" s="52" t="str">
         <f aca="true">IF(I196="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="49"/>
-      <c r="C197" s="49"/>
-      <c r="E197" s="50"/>
-      <c r="F197" s="50"/>
-      <c r="H197" s="52" t="str">
+      <c r="B197" s="37"/>
+      <c r="C197" s="37"/>
+      <c r="E197" s="49"/>
+      <c r="F197" s="49"/>
+      <c r="H197" s="51" t="str">
         <f aca="true">IF(I197 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q197" s="53"/>
-      <c r="R197" s="53" t="str">
+      <c r="Q197" s="52"/>
+      <c r="R197" s="52" t="str">
         <f aca="true">IF(I197="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="49"/>
-      <c r="C198" s="49"/>
-      <c r="E198" s="50"/>
-      <c r="F198" s="50"/>
-      <c r="H198" s="52" t="str">
+      <c r="B198" s="37"/>
+      <c r="C198" s="37"/>
+      <c r="E198" s="49"/>
+      <c r="F198" s="49"/>
+      <c r="H198" s="51" t="str">
         <f aca="true">IF(I198 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q198" s="53"/>
-      <c r="R198" s="53" t="str">
+      <c r="Q198" s="52"/>
+      <c r="R198" s="52" t="str">
         <f aca="true">IF(I198="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="49"/>
-      <c r="C199" s="49"/>
-      <c r="E199" s="50"/>
-      <c r="F199" s="50"/>
-      <c r="H199" s="52" t="str">
+      <c r="B199" s="37"/>
+      <c r="C199" s="37"/>
+      <c r="E199" s="49"/>
+      <c r="F199" s="49"/>
+      <c r="H199" s="51" t="str">
         <f aca="true">IF(I199 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q199" s="53"/>
-      <c r="R199" s="53" t="str">
+      <c r="Q199" s="52"/>
+      <c r="R199" s="52" t="str">
         <f aca="true">IF(I199="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="49"/>
-      <c r="C200" s="49"/>
-      <c r="E200" s="50"/>
-      <c r="F200" s="50"/>
-      <c r="H200" s="52" t="str">
+      <c r="B200" s="37"/>
+      <c r="C200" s="37"/>
+      <c r="E200" s="49"/>
+      <c r="F200" s="49"/>
+      <c r="H200" s="51" t="str">
         <f aca="true">IF(I200 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q200" s="53"/>
-      <c r="R200" s="53" t="str">
+      <c r="Q200" s="52"/>
+      <c r="R200" s="52" t="str">
         <f aca="true">IF(I200="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B201" s="49"/>
-      <c r="C201" s="49"/>
-      <c r="E201" s="50"/>
-      <c r="F201" s="50"/>
-      <c r="H201" s="52" t="str">
+      <c r="B201" s="37"/>
+      <c r="C201" s="37"/>
+      <c r="E201" s="49"/>
+      <c r="F201" s="49"/>
+      <c r="H201" s="51" t="str">
         <f aca="true">IF(I201 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q201" s="53"/>
-      <c r="R201" s="53" t="str">
+      <c r="Q201" s="52"/>
+      <c r="R201" s="52" t="str">
         <f aca="true">IF(I201="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B202" s="49"/>
-      <c r="C202" s="49"/>
-      <c r="E202" s="50"/>
-      <c r="F202" s="50"/>
-      <c r="H202" s="52" t="str">
+      <c r="B202" s="37"/>
+      <c r="C202" s="37"/>
+      <c r="E202" s="49"/>
+      <c r="F202" s="49"/>
+      <c r="H202" s="51" t="str">
         <f aca="true">IF(I202 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q202" s="53"/>
-      <c r="R202" s="53" t="str">
+      <c r="Q202" s="52"/>
+      <c r="R202" s="52" t="str">
         <f aca="true">IF(I202="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B203" s="49"/>
-      <c r="C203" s="49"/>
-      <c r="E203" s="50"/>
-      <c r="F203" s="50"/>
-      <c r="H203" s="52" t="str">
+      <c r="B203" s="37"/>
+      <c r="C203" s="37"/>
+      <c r="E203" s="49"/>
+      <c r="F203" s="49"/>
+      <c r="H203" s="51" t="str">
         <f aca="true">IF(I203 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q203" s="53"/>
-      <c r="R203" s="53" t="str">
+      <c r="Q203" s="52"/>
+      <c r="R203" s="52" t="str">
         <f aca="true">IF(I203="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B204" s="49"/>
-      <c r="C204" s="49"/>
-      <c r="E204" s="50"/>
-      <c r="F204" s="50"/>
-      <c r="H204" s="52" t="str">
+      <c r="B204" s="37"/>
+      <c r="C204" s="37"/>
+      <c r="E204" s="49"/>
+      <c r="F204" s="49"/>
+      <c r="H204" s="51" t="str">
         <f aca="true">IF(I204 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q204" s="53"/>
-      <c r="R204" s="53" t="str">
+      <c r="Q204" s="52"/>
+      <c r="R204" s="52" t="str">
         <f aca="true">IF(I204="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B205" s="49"/>
-      <c r="C205" s="49"/>
-      <c r="E205" s="50"/>
-      <c r="F205" s="50"/>
-      <c r="H205" s="52" t="str">
+      <c r="B205" s="37"/>
+      <c r="C205" s="37"/>
+      <c r="E205" s="49"/>
+      <c r="F205" s="49"/>
+      <c r="H205" s="51" t="str">
         <f aca="true">IF(I205 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q205" s="53"/>
-      <c r="R205" s="53" t="str">
+      <c r="Q205" s="52"/>
+      <c r="R205" s="52" t="str">
         <f aca="true">IF(I205="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B206" s="49"/>
-      <c r="C206" s="49"/>
-      <c r="E206" s="50"/>
-      <c r="F206" s="50"/>
-      <c r="H206" s="52" t="str">
+      <c r="B206" s="37"/>
+      <c r="C206" s="37"/>
+      <c r="E206" s="49"/>
+      <c r="F206" s="49"/>
+      <c r="H206" s="51" t="str">
         <f aca="true">IF(I206 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q206" s="53"/>
-      <c r="R206" s="53" t="str">
+      <c r="Q206" s="52"/>
+      <c r="R206" s="52" t="str">
         <f aca="true">IF(I206="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B207" s="49"/>
-      <c r="C207" s="49"/>
-      <c r="E207" s="50"/>
-      <c r="F207" s="50"/>
-      <c r="H207" s="52" t="str">
+      <c r="B207" s="37"/>
+      <c r="C207" s="37"/>
+      <c r="E207" s="49"/>
+      <c r="F207" s="49"/>
+      <c r="H207" s="51" t="str">
         <f aca="true">IF(I207 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q207" s="53"/>
-      <c r="R207" s="53" t="str">
+      <c r="Q207" s="52"/>
+      <c r="R207" s="52" t="str">
         <f aca="true">IF(I207="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B208" s="49"/>
-      <c r="C208" s="49"/>
-      <c r="E208" s="50"/>
-      <c r="H208" s="52" t="str">
+      <c r="B208" s="37"/>
+      <c r="C208" s="37"/>
+      <c r="E208" s="49"/>
+      <c r="H208" s="51" t="str">
         <f aca="true">IF(I208 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q208" s="53"/>
-      <c r="R208" s="53" t="str">
+      <c r="Q208" s="52"/>
+      <c r="R208" s="52" t="str">
         <f aca="true">IF(I208="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B209" s="49"/>
-      <c r="C209" s="49"/>
-      <c r="E209" s="50"/>
-      <c r="H209" s="52" t="str">
+      <c r="B209" s="37"/>
+      <c r="C209" s="37"/>
+      <c r="E209" s="49"/>
+      <c r="H209" s="51" t="str">
         <f aca="true">IF(I209 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q209" s="53"/>
-      <c r="R209" s="53" t="str">
+      <c r="Q209" s="52"/>
+      <c r="R209" s="52" t="str">
         <f aca="true">IF(I209="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B210" s="49"/>
-      <c r="C210" s="49"/>
-      <c r="E210" s="50"/>
-      <c r="H210" s="52" t="str">
+      <c r="B210" s="37"/>
+      <c r="C210" s="37"/>
+      <c r="E210" s="49"/>
+      <c r="H210" s="51" t="str">
         <f aca="true">IF(I210 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q210" s="53"/>
-      <c r="R210" s="53" t="str">
+      <c r="Q210" s="52"/>
+      <c r="R210" s="52" t="str">
         <f aca="true">IF(I210="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B211" s="49"/>
-      <c r="C211" s="49"/>
-      <c r="E211" s="50"/>
-      <c r="H211" s="52" t="str">
+      <c r="B211" s="37"/>
+      <c r="C211" s="37"/>
+      <c r="E211" s="49"/>
+      <c r="H211" s="51" t="str">
         <f aca="true">IF(I211 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q211" s="53"/>
-      <c r="R211" s="53" t="str">
+      <c r="Q211" s="52"/>
+      <c r="R211" s="52" t="str">
         <f aca="true">IF(I211="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B212" s="49"/>
-      <c r="C212" s="49"/>
-      <c r="E212" s="50"/>
-      <c r="H212" s="52" t="str">
+      <c r="B212" s="37"/>
+      <c r="C212" s="37"/>
+      <c r="E212" s="49"/>
+      <c r="H212" s="51" t="str">
         <f aca="true">IF(I212 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q212" s="53"/>
-      <c r="R212" s="53" t="str">
+      <c r="Q212" s="52"/>
+      <c r="R212" s="52" t="str">
         <f aca="true">IF(I212="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B213" s="49"/>
-      <c r="C213" s="49"/>
-      <c r="E213" s="50"/>
-      <c r="H213" s="52" t="str">
+      <c r="B213" s="37"/>
+      <c r="C213" s="37"/>
+      <c r="E213" s="49"/>
+      <c r="H213" s="51" t="str">
         <f aca="true">IF(I213 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q213" s="53"/>
-      <c r="R213" s="53" t="str">
+      <c r="Q213" s="52"/>
+      <c r="R213" s="52" t="str">
         <f aca="true">IF(I213="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B214" s="49"/>
-      <c r="C214" s="49"/>
-      <c r="E214" s="50"/>
-      <c r="H214" s="52" t="str">
+      <c r="B214" s="37"/>
+      <c r="C214" s="37"/>
+      <c r="E214" s="49"/>
+      <c r="H214" s="51" t="str">
         <f aca="true">IF(I214 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q214" s="53"/>
-      <c r="R214" s="53" t="str">
+      <c r="Q214" s="52"/>
+      <c r="R214" s="52" t="str">
         <f aca="true">IF(I214="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B215" s="49"/>
-      <c r="C215" s="49"/>
-      <c r="E215" s="50"/>
-      <c r="H215" s="52" t="str">
+      <c r="B215" s="37"/>
+      <c r="C215" s="37"/>
+      <c r="E215" s="49"/>
+      <c r="H215" s="51" t="str">
         <f aca="true">IF(I215 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q215" s="53"/>
-      <c r="R215" s="53" t="str">
+      <c r="Q215" s="52"/>
+      <c r="R215" s="52" t="str">
         <f aca="true">IF(I215="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B216" s="49"/>
-      <c r="C216" s="49"/>
-      <c r="E216" s="50"/>
-      <c r="H216" s="52" t="str">
+      <c r="B216" s="37"/>
+      <c r="C216" s="37"/>
+      <c r="E216" s="49"/>
+      <c r="H216" s="51" t="str">
         <f aca="true">IF(I216 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q216" s="53"/>
-      <c r="R216" s="53" t="str">
+      <c r="Q216" s="52"/>
+      <c r="R216" s="52" t="str">
         <f aca="true">IF(I216="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B217" s="49"/>
-      <c r="C217" s="49"/>
-      <c r="E217" s="50"/>
-      <c r="H217" s="52" t="str">
+      <c r="B217" s="37"/>
+      <c r="C217" s="37"/>
+      <c r="E217" s="49"/>
+      <c r="H217" s="51" t="str">
         <f aca="true">IF(I217 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q217" s="53"/>
-      <c r="R217" s="53" t="str">
+      <c r="Q217" s="52"/>
+      <c r="R217" s="52" t="str">
         <f aca="true">IF(I217="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B218" s="49"/>
-      <c r="C218" s="49"/>
-      <c r="E218" s="50"/>
-      <c r="H218" s="52" t="str">
+      <c r="B218" s="37"/>
+      <c r="C218" s="37"/>
+      <c r="E218" s="49"/>
+      <c r="H218" s="51" t="str">
         <f aca="true">IF(I218 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q218" s="53"/>
-      <c r="R218" s="53" t="str">
+      <c r="Q218" s="52"/>
+      <c r="R218" s="52" t="str">
         <f aca="true">IF(I218="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B219" s="49"/>
-      <c r="C219" s="49"/>
-      <c r="E219" s="50"/>
-      <c r="H219" s="52" t="str">
+      <c r="B219" s="37"/>
+      <c r="C219" s="37"/>
+      <c r="E219" s="49"/>
+      <c r="H219" s="51" t="str">
         <f aca="true">IF(I219 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q219" s="53"/>
-      <c r="R219" s="53" t="str">
+      <c r="Q219" s="52"/>
+      <c r="R219" s="52" t="str">
         <f aca="true">IF(I219="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B220" s="49"/>
-      <c r="C220" s="49"/>
-      <c r="E220" s="50"/>
-      <c r="H220" s="52" t="str">
+      <c r="B220" s="37"/>
+      <c r="C220" s="37"/>
+      <c r="E220" s="49"/>
+      <c r="H220" s="51" t="str">
         <f aca="true">IF(I220 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q220" s="53"/>
-      <c r="R220" s="53" t="str">
+      <c r="Q220" s="52"/>
+      <c r="R220" s="52" t="str">
         <f aca="true">IF(I220="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B221" s="49"/>
-      <c r="C221" s="49"/>
-      <c r="E221" s="50"/>
-      <c r="H221" s="52" t="str">
+      <c r="B221" s="37"/>
+      <c r="C221" s="37"/>
+      <c r="E221" s="49"/>
+      <c r="H221" s="51" t="str">
         <f aca="true">IF(I221 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q221" s="53"/>
-      <c r="R221" s="53" t="str">
+      <c r="Q221" s="52"/>
+      <c r="R221" s="52" t="str">
         <f aca="true">IF(I221="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B222" s="49"/>
-      <c r="C222" s="49"/>
-      <c r="E222" s="50"/>
-      <c r="H222" s="52" t="str">
+      <c r="B222" s="37"/>
+      <c r="C222" s="37"/>
+      <c r="E222" s="49"/>
+      <c r="H222" s="51" t="str">
         <f aca="true">IF(I222 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q222" s="53"/>
-      <c r="R222" s="53" t="str">
+      <c r="Q222" s="52"/>
+      <c r="R222" s="52" t="str">
         <f aca="true">IF(I222="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B223" s="49"/>
-      <c r="C223" s="49"/>
-      <c r="E223" s="50"/>
-      <c r="H223" s="52" t="str">
+      <c r="B223" s="37"/>
+      <c r="C223" s="37"/>
+      <c r="E223" s="49"/>
+      <c r="H223" s="51" t="str">
         <f aca="true">IF(I223 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q223" s="53"/>
-      <c r="R223" s="53" t="str">
+      <c r="Q223" s="52"/>
+      <c r="R223" s="52" t="str">
         <f aca="true">IF(I223="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B224" s="49"/>
-      <c r="C224" s="49"/>
-      <c r="E224" s="50"/>
-      <c r="H224" s="52" t="str">
+      <c r="B224" s="37"/>
+      <c r="C224" s="37"/>
+      <c r="E224" s="49"/>
+      <c r="H224" s="51" t="str">
         <f aca="true">IF(I224 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q224" s="53"/>
-      <c r="R224" s="53" t="str">
+      <c r="Q224" s="52"/>
+      <c r="R224" s="52" t="str">
         <f aca="true">IF(I224="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B225" s="49"/>
-      <c r="C225" s="49"/>
-      <c r="E225" s="50"/>
-      <c r="H225" s="52" t="str">
+      <c r="B225" s="37"/>
+      <c r="C225" s="37"/>
+      <c r="E225" s="49"/>
+      <c r="H225" s="51" t="str">
         <f aca="true">IF(I225 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q225" s="53"/>
-      <c r="R225" s="53" t="str">
+      <c r="Q225" s="52"/>
+      <c r="R225" s="52" t="str">
         <f aca="true">IF(I225="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B226" s="49"/>
-      <c r="C226" s="49"/>
-      <c r="E226" s="50"/>
-      <c r="H226" s="52" t="str">
+      <c r="B226" s="37"/>
+      <c r="C226" s="37"/>
+      <c r="E226" s="49"/>
+      <c r="H226" s="51" t="str">
         <f aca="true">IF(I226 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q226" s="53"/>
-      <c r="R226" s="53" t="str">
+      <c r="Q226" s="52"/>
+      <c r="R226" s="52" t="str">
         <f aca="true">IF(I226="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B227" s="49"/>
-      <c r="C227" s="49"/>
-      <c r="E227" s="50"/>
-      <c r="H227" s="52" t="str">
+      <c r="B227" s="37"/>
+      <c r="C227" s="37"/>
+      <c r="E227" s="49"/>
+      <c r="H227" s="51" t="str">
         <f aca="true">IF(I227 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q227" s="53"/>
-      <c r="R227" s="53" t="str">
+      <c r="Q227" s="52"/>
+      <c r="R227" s="52" t="str">
         <f aca="true">IF(I227="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B228" s="49"/>
-      <c r="C228" s="49"/>
-      <c r="E228" s="50"/>
-      <c r="H228" s="52" t="str">
+      <c r="B228" s="37"/>
+      <c r="C228" s="37"/>
+      <c r="E228" s="49"/>
+      <c r="H228" s="51" t="str">
         <f aca="true">IF(I228 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q228" s="53"/>
-      <c r="R228" s="53"/>
+      <c r="Q228" s="52"/>
+      <c r="R228" s="52"/>
     </row>
     <row r="229" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B229" s="49"/>
-      <c r="C229" s="49"/>
-      <c r="E229" s="50"/>
-      <c r="H229" s="52" t="str">
+      <c r="B229" s="37"/>
+      <c r="C229" s="37"/>
+      <c r="E229" s="49"/>
+      <c r="H229" s="51" t="str">
         <f aca="true">IF(I229 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q229" s="53"/>
-      <c r="R229" s="53"/>
+      <c r="Q229" s="52"/>
+      <c r="R229" s="52"/>
     </row>
     <row r="230" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B230" s="49"/>
-      <c r="C230" s="49"/>
-      <c r="E230" s="50"/>
-      <c r="H230" s="52" t="str">
+      <c r="B230" s="37"/>
+      <c r="C230" s="37"/>
+      <c r="E230" s="49"/>
+      <c r="H230" s="51" t="str">
         <f aca="true">IF(I230 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q230" s="53"/>
-      <c r="R230" s="53"/>
+      <c r="Q230" s="52"/>
+      <c r="R230" s="52"/>
     </row>
     <row r="231" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B231" s="49"/>
-      <c r="C231" s="49"/>
-      <c r="E231" s="50"/>
-      <c r="H231" s="52" t="str">
+      <c r="B231" s="37"/>
+      <c r="C231" s="37"/>
+      <c r="E231" s="49"/>
+      <c r="H231" s="51" t="str">
         <f aca="true">IF(I231 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q231" s="53"/>
-      <c r="R231" s="53"/>
+      <c r="Q231" s="52"/>
+      <c r="R231" s="52"/>
     </row>
     <row r="232" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B232" s="49"/>
-      <c r="C232" s="49"/>
-      <c r="E232" s="50"/>
-      <c r="H232" s="52" t="str">
+      <c r="B232" s="37"/>
+      <c r="C232" s="37"/>
+      <c r="E232" s="49"/>
+      <c r="H232" s="51" t="str">
         <f aca="true">IF(I232 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q232" s="53"/>
-      <c r="R232" s="53"/>
+      <c r="Q232" s="52"/>
+      <c r="R232" s="52"/>
     </row>
     <row r="233" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B233" s="49"/>
-      <c r="C233" s="49"/>
-      <c r="E233" s="50"/>
-      <c r="H233" s="52" t="str">
+      <c r="B233" s="37"/>
+      <c r="C233" s="37"/>
+      <c r="E233" s="49"/>
+      <c r="H233" s="51" t="str">
         <f aca="true">IF(I233 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q233" s="53"/>
-      <c r="R233" s="53"/>
+      <c r="Q233" s="52"/>
+      <c r="R233" s="52"/>
     </row>
     <row r="234" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B234" s="49"/>
-      <c r="C234" s="49"/>
-      <c r="E234" s="50"/>
-      <c r="H234" s="52" t="str">
+      <c r="B234" s="37"/>
+      <c r="C234" s="37"/>
+      <c r="E234" s="49"/>
+      <c r="H234" s="51" t="str">
         <f aca="true">IF(I234 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q234" s="53"/>
-      <c r="R234" s="53"/>
+      <c r="Q234" s="52"/>
+      <c r="R234" s="52"/>
     </row>
     <row r="235" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B235" s="49"/>
-      <c r="C235" s="49"/>
-      <c r="E235" s="50"/>
-      <c r="H235" s="52" t="str">
+      <c r="B235" s="37"/>
+      <c r="C235" s="37"/>
+      <c r="E235" s="49"/>
+      <c r="H235" s="51" t="str">
         <f aca="true">IF(I235 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q235" s="53"/>
-      <c r="R235" s="53"/>
+      <c r="Q235" s="52"/>
+      <c r="R235" s="52"/>
     </row>
     <row r="236" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B236" s="49"/>
-      <c r="C236" s="49"/>
-      <c r="E236" s="50"/>
-      <c r="H236" s="52" t="str">
+      <c r="B236" s="37"/>
+      <c r="C236" s="37"/>
+      <c r="E236" s="49"/>
+      <c r="H236" s="51" t="str">
         <f aca="true">IF(I236 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q236" s="53"/>
-      <c r="R236" s="53"/>
+      <c r="Q236" s="52"/>
+      <c r="R236" s="52"/>
     </row>
     <row r="237" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B237" s="49"/>
-      <c r="C237" s="49"/>
-      <c r="E237" s="50"/>
-      <c r="H237" s="52" t="str">
+      <c r="B237" s="37"/>
+      <c r="C237" s="37"/>
+      <c r="E237" s="49"/>
+      <c r="H237" s="51" t="str">
         <f aca="true">IF(I237 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q237" s="53"/>
-      <c r="R237" s="53"/>
+      <c r="Q237" s="52"/>
+      <c r="R237" s="52"/>
     </row>
     <row r="238" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B238" s="49"/>
-      <c r="C238" s="49"/>
-      <c r="E238" s="50"/>
-      <c r="H238" s="52" t="str">
+      <c r="B238" s="37"/>
+      <c r="C238" s="37"/>
+      <c r="E238" s="49"/>
+      <c r="H238" s="51" t="str">
         <f aca="true">IF(I238 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q238" s="53"/>
-      <c r="R238" s="53"/>
+      <c r="Q238" s="52"/>
+      <c r="R238" s="52"/>
     </row>
     <row r="239" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B239" s="49"/>
-      <c r="C239" s="49"/>
-      <c r="E239" s="50"/>
-      <c r="H239" s="52" t="str">
+      <c r="B239" s="37"/>
+      <c r="C239" s="37"/>
+      <c r="E239" s="49"/>
+      <c r="H239" s="51" t="str">
         <f aca="true">IF(I239 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q239" s="53"/>
-      <c r="R239" s="53"/>
+      <c r="Q239" s="52"/>
+      <c r="R239" s="52"/>
     </row>
     <row r="240" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B240" s="49"/>
-      <c r="C240" s="49"/>
-      <c r="E240" s="50"/>
-      <c r="H240" s="52" t="str">
+      <c r="B240" s="37"/>
+      <c r="C240" s="37"/>
+      <c r="E240" s="49"/>
+      <c r="H240" s="51" t="str">
         <f aca="true">IF(I240 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q240" s="53"/>
-      <c r="R240" s="53"/>
+      <c r="Q240" s="52"/>
+      <c r="R240" s="52"/>
     </row>
     <row r="241" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B241" s="49"/>
-      <c r="C241" s="49"/>
-      <c r="E241" s="50"/>
-      <c r="H241" s="52" t="str">
+      <c r="B241" s="37"/>
+      <c r="C241" s="37"/>
+      <c r="E241" s="49"/>
+      <c r="H241" s="51" t="str">
         <f aca="true">IF(I241 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q241" s="53"/>
-      <c r="R241" s="53"/>
+      <c r="Q241" s="52"/>
+      <c r="R241" s="52"/>
     </row>
     <row r="242" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B242" s="49"/>
-      <c r="C242" s="49"/>
-      <c r="E242" s="50"/>
-      <c r="H242" s="52" t="str">
+      <c r="B242" s="37"/>
+      <c r="C242" s="37"/>
+      <c r="E242" s="49"/>
+      <c r="H242" s="51" t="str">
         <f aca="true">IF(I242 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q242" s="53"/>
-      <c r="R242" s="53"/>
+      <c r="Q242" s="52"/>
+      <c r="R242" s="52"/>
     </row>
     <row r="243" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B243" s="49"/>
-      <c r="C243" s="49"/>
-      <c r="E243" s="50"/>
-      <c r="H243" s="52" t="str">
+      <c r="B243" s="37"/>
+      <c r="C243" s="37"/>
+      <c r="E243" s="49"/>
+      <c r="H243" s="51" t="str">
         <f aca="true">IF(I243 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q243" s="53"/>
-      <c r="R243" s="53"/>
+      <c r="Q243" s="52"/>
+      <c r="R243" s="52"/>
     </row>
     <row r="244" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B244" s="49"/>
-      <c r="C244" s="49"/>
-      <c r="E244" s="50"/>
-      <c r="H244" s="52" t="str">
+      <c r="B244" s="37"/>
+      <c r="C244" s="37"/>
+      <c r="E244" s="49"/>
+      <c r="H244" s="51" t="str">
         <f aca="true">IF(I244 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q244" s="53"/>
-      <c r="R244" s="53"/>
+      <c r="Q244" s="52"/>
+      <c r="R244" s="52"/>
     </row>
     <row r="245" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B245" s="49"/>
-      <c r="C245" s="49"/>
-      <c r="E245" s="50"/>
-      <c r="H245" s="52" t="str">
+      <c r="B245" s="37"/>
+      <c r="C245" s="37"/>
+      <c r="E245" s="49"/>
+      <c r="H245" s="51" t="str">
         <f aca="true">IF(I245 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q245" s="53"/>
-      <c r="R245" s="53"/>
+      <c r="Q245" s="52"/>
+      <c r="R245" s="52"/>
     </row>
     <row r="246" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B246" s="49"/>
-      <c r="C246" s="49"/>
-      <c r="E246" s="50"/>
-      <c r="H246" s="52" t="str">
+      <c r="B246" s="37"/>
+      <c r="C246" s="37"/>
+      <c r="E246" s="49"/>
+      <c r="H246" s="51" t="str">
         <f aca="true">IF(I246 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q246" s="53"/>
-      <c r="R246" s="53"/>
+      <c r="Q246" s="52"/>
+      <c r="R246" s="52"/>
     </row>
     <row r="247" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B247" s="49"/>
-      <c r="C247" s="49"/>
-      <c r="E247" s="50"/>
-      <c r="H247" s="52" t="str">
+      <c r="B247" s="37"/>
+      <c r="C247" s="37"/>
+      <c r="E247" s="49"/>
+      <c r="H247" s="51" t="str">
         <f aca="true">IF(I247 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q247" s="53"/>
-      <c r="R247" s="53"/>
+      <c r="Q247" s="52"/>
+      <c r="R247" s="52"/>
     </row>
     <row r="248" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B248" s="49"/>
-      <c r="C248" s="49"/>
-      <c r="E248" s="50"/>
-      <c r="H248" s="52" t="str">
+      <c r="B248" s="37"/>
+      <c r="C248" s="37"/>
+      <c r="E248" s="49"/>
+      <c r="H248" s="51" t="str">
         <f aca="true">IF(I248 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q248" s="53"/>
-      <c r="R248" s="53"/>
+      <c r="Q248" s="52"/>
+      <c r="R248" s="52"/>
     </row>
     <row r="249" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B249" s="49"/>
-      <c r="C249" s="49"/>
-      <c r="E249" s="50"/>
-      <c r="H249" s="52" t="str">
+      <c r="B249" s="37"/>
+      <c r="C249" s="37"/>
+      <c r="E249" s="49"/>
+      <c r="H249" s="51" t="str">
         <f aca="true">IF(I249 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q249" s="53"/>
-      <c r="R249" s="53"/>
+      <c r="Q249" s="52"/>
+      <c r="R249" s="52"/>
     </row>
     <row r="250" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B250" s="49"/>
-      <c r="C250" s="49"/>
-      <c r="E250" s="50"/>
-      <c r="H250" s="52" t="str">
+      <c r="B250" s="37"/>
+      <c r="C250" s="37"/>
+      <c r="E250" s="49"/>
+      <c r="H250" s="51" t="str">
         <f aca="true">IF(I250 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q250" s="53"/>
-      <c r="R250" s="53"/>
+      <c r="Q250" s="52"/>
+      <c r="R250" s="52"/>
     </row>
     <row r="251" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B251" s="49"/>
-      <c r="C251" s="49"/>
-      <c r="E251" s="50"/>
-      <c r="H251" s="52" t="str">
+      <c r="B251" s="37"/>
+      <c r="C251" s="37"/>
+      <c r="E251" s="49"/>
+      <c r="H251" s="51" t="str">
         <f aca="true">IF(I251 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q251" s="53"/>
-      <c r="R251" s="53"/>
+      <c r="Q251" s="52"/>
+      <c r="R251" s="52"/>
     </row>
     <row r="252" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B252" s="49"/>
-      <c r="C252" s="49"/>
-      <c r="E252" s="50"/>
-      <c r="H252" s="52" t="str">
+      <c r="B252" s="37"/>
+      <c r="C252" s="37"/>
+      <c r="E252" s="49"/>
+      <c r="H252" s="51" t="str">
         <f aca="true">IF(I252 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q252" s="53"/>
-      <c r="R252" s="53"/>
+      <c r="Q252" s="52"/>
+      <c r="R252" s="52"/>
     </row>
     <row r="253" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B253" s="49"/>
-      <c r="C253" s="49"/>
-      <c r="E253" s="50"/>
-      <c r="H253" s="52" t="str">
+      <c r="B253" s="37"/>
+      <c r="C253" s="37"/>
+      <c r="E253" s="49"/>
+      <c r="H253" s="51" t="str">
         <f aca="true">IF(I253 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q253" s="53"/>
-      <c r="R253" s="53"/>
+      <c r="Q253" s="52"/>
+      <c r="R253" s="52"/>
     </row>
     <row r="254" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B254" s="49"/>
-      <c r="C254" s="49"/>
-      <c r="E254" s="50"/>
-      <c r="H254" s="52" t="str">
+      <c r="B254" s="37"/>
+      <c r="C254" s="37"/>
+      <c r="E254" s="49"/>
+      <c r="H254" s="51" t="str">
         <f aca="true">IF(I254 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q254" s="53"/>
-      <c r="R254" s="53"/>
+      <c r="Q254" s="52"/>
+      <c r="R254" s="52"/>
     </row>
     <row r="255" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B255" s="49"/>
-      <c r="C255" s="49"/>
-      <c r="E255" s="50"/>
-      <c r="H255" s="52" t="str">
+      <c r="B255" s="37"/>
+      <c r="C255" s="37"/>
+      <c r="E255" s="49"/>
+      <c r="H255" s="51" t="str">
         <f aca="true">IF(I255 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q255" s="53"/>
-      <c r="R255" s="53"/>
+      <c r="Q255" s="52"/>
+      <c r="R255" s="52"/>
     </row>
     <row r="256" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B256" s="49"/>
-      <c r="C256" s="49"/>
-      <c r="E256" s="50"/>
-      <c r="H256" s="52" t="str">
+      <c r="B256" s="37"/>
+      <c r="C256" s="37"/>
+      <c r="E256" s="49"/>
+      <c r="H256" s="51" t="str">
         <f aca="true">IF(I256 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q256" s="53"/>
-      <c r="R256" s="53"/>
+      <c r="Q256" s="52"/>
+      <c r="R256" s="52"/>
     </row>
     <row r="257" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B257" s="49"/>
-      <c r="C257" s="49"/>
-      <c r="E257" s="50"/>
-      <c r="H257" s="52" t="str">
+      <c r="B257" s="37"/>
+      <c r="C257" s="37"/>
+      <c r="E257" s="49"/>
+      <c r="H257" s="51" t="str">
         <f aca="true">IF(I257 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q257" s="53"/>
-      <c r="R257" s="53"/>
+      <c r="Q257" s="52"/>
+      <c r="R257" s="52"/>
     </row>
     <row r="258" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B258" s="49"/>
-      <c r="C258" s="49"/>
-      <c r="E258" s="50"/>
-      <c r="H258" s="52" t="str">
+      <c r="B258" s="37"/>
+      <c r="C258" s="37"/>
+      <c r="E258" s="49"/>
+      <c r="H258" s="51" t="str">
         <f aca="true">IF(I258 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q258" s="53"/>
-      <c r="R258" s="53"/>
+      <c r="Q258" s="52"/>
+      <c r="R258" s="52"/>
     </row>
     <row r="259" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B259" s="49"/>
-      <c r="C259" s="49"/>
-      <c r="E259" s="50"/>
-      <c r="H259" s="52" t="str">
+      <c r="B259" s="37"/>
+      <c r="C259" s="37"/>
+      <c r="E259" s="49"/>
+      <c r="H259" s="51" t="str">
         <f aca="true">IF(I259 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q259" s="53"/>
-      <c r="R259" s="53"/>
+      <c r="Q259" s="52"/>
+      <c r="R259" s="52"/>
     </row>
     <row r="260" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B260" s="49"/>
-      <c r="C260" s="49"/>
-      <c r="E260" s="50"/>
-      <c r="H260" s="52" t="str">
+      <c r="B260" s="37"/>
+      <c r="C260" s="37"/>
+      <c r="E260" s="49"/>
+      <c r="H260" s="51" t="str">
         <f aca="true">IF(I260 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q260" s="53"/>
-      <c r="R260" s="53"/>
+      <c r="Q260" s="52"/>
+      <c r="R260" s="52"/>
     </row>
     <row r="261" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B261" s="49"/>
-      <c r="C261" s="49"/>
-      <c r="E261" s="50"/>
-      <c r="H261" s="52" t="str">
+      <c r="B261" s="37"/>
+      <c r="C261" s="37"/>
+      <c r="E261" s="49"/>
+      <c r="H261" s="51" t="str">
         <f aca="true">IF(I261 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q261" s="53"/>
-      <c r="R261" s="53"/>
+      <c r="Q261" s="52"/>
+      <c r="R261" s="52"/>
     </row>
     <row r="262" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B262" s="49"/>
-      <c r="C262" s="49"/>
-      <c r="E262" s="50"/>
-      <c r="H262" s="52" t="str">
+      <c r="B262" s="37"/>
+      <c r="C262" s="37"/>
+      <c r="E262" s="49"/>
+      <c r="H262" s="51" t="str">
         <f aca="true">IF(I262 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q262" s="53"/>
-      <c r="R262" s="53"/>
+      <c r="Q262" s="52"/>
+      <c r="R262" s="52"/>
     </row>
     <row r="263" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B263" s="49"/>
-      <c r="C263" s="49"/>
-      <c r="E263" s="50"/>
-      <c r="H263" s="52" t="str">
+      <c r="B263" s="37"/>
+      <c r="C263" s="37"/>
+      <c r="E263" s="49"/>
+      <c r="H263" s="51" t="str">
         <f aca="true">IF(I263 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q263" s="53"/>
-      <c r="R263" s="53"/>
+      <c r="Q263" s="52"/>
+      <c r="R263" s="52"/>
     </row>
     <row r="264" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B264" s="49"/>
-      <c r="C264" s="49"/>
-      <c r="E264" s="50"/>
-      <c r="H264" s="52" t="str">
+      <c r="B264" s="37"/>
+      <c r="C264" s="37"/>
+      <c r="E264" s="49"/>
+      <c r="H264" s="51" t="str">
         <f aca="true">IF(I264 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q264" s="53"/>
-      <c r="R264" s="53"/>
+      <c r="Q264" s="52"/>
+      <c r="R264" s="52"/>
     </row>
     <row r="265" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B265" s="49"/>
-      <c r="C265" s="49"/>
-      <c r="E265" s="50"/>
-      <c r="H265" s="52" t="str">
+      <c r="B265" s="37"/>
+      <c r="C265" s="37"/>
+      <c r="E265" s="49"/>
+      <c r="H265" s="51" t="str">
         <f aca="true">IF(I265 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q265" s="53"/>
-      <c r="R265" s="53"/>
+      <c r="Q265" s="52"/>
+      <c r="R265" s="52"/>
     </row>
     <row r="266" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B266" s="49"/>
-      <c r="C266" s="49"/>
-      <c r="E266" s="50"/>
-      <c r="H266" s="52" t="str">
+      <c r="B266" s="37"/>
+      <c r="C266" s="37"/>
+      <c r="E266" s="49"/>
+      <c r="H266" s="51" t="str">
         <f aca="true">IF(I266 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B267" s="49"/>
-      <c r="C267" s="49"/>
-      <c r="E267" s="50"/>
-      <c r="H267" s="52" t="str">
+      <c r="B267" s="37"/>
+      <c r="C267" s="37"/>
+      <c r="E267" s="49"/>
+      <c r="H267" s="51" t="str">
         <f aca="true">IF(I267 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B268" s="49"/>
-      <c r="C268" s="49"/>
-      <c r="E268" s="50"/>
-      <c r="H268" s="52" t="str">
+      <c r="B268" s="37"/>
+      <c r="C268" s="37"/>
+      <c r="E268" s="49"/>
+      <c r="H268" s="51" t="str">
         <f aca="true">IF(I268 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B269" s="49"/>
-      <c r="C269" s="49"/>
-      <c r="E269" s="50"/>
-      <c r="H269" s="52" t="str">
+      <c r="B269" s="37"/>
+      <c r="C269" s="37"/>
+      <c r="E269" s="49"/>
+      <c r="H269" s="51" t="str">
         <f aca="true">IF(I269 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B270" s="49"/>
-      <c r="C270" s="49"/>
-      <c r="E270" s="50"/>
-      <c r="H270" s="52" t="str">
+      <c r="B270" s="37"/>
+      <c r="C270" s="37"/>
+      <c r="E270" s="49"/>
+      <c r="H270" s="51" t="str">
         <f aca="true">IF(I270 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B271" s="49"/>
-      <c r="C271" s="49"/>
-      <c r="E271" s="50"/>
-      <c r="H271" s="52" t="str">
+      <c r="B271" s="37"/>
+      <c r="C271" s="37"/>
+      <c r="E271" s="49"/>
+      <c r="H271" s="51" t="str">
         <f aca="true">IF(I271 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B272" s="49"/>
-      <c r="C272" s="49"/>
-      <c r="E272" s="50"/>
-      <c r="H272" s="52" t="str">
+      <c r="B272" s="37"/>
+      <c r="C272" s="37"/>
+      <c r="E272" s="49"/>
+      <c r="H272" s="51" t="str">
         <f aca="true">IF(I272 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B273" s="49"/>
-      <c r="C273" s="49"/>
-      <c r="E273" s="50"/>
-      <c r="H273" s="52" t="str">
+      <c r="B273" s="37"/>
+      <c r="C273" s="37"/>
+      <c r="E273" s="49"/>
+      <c r="H273" s="51" t="str">
         <f aca="true">IF(I273 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B274" s="49"/>
-      <c r="C274" s="49"/>
-      <c r="E274" s="50"/>
-      <c r="H274" s="52" t="str">
+      <c r="B274" s="37"/>
+      <c r="C274" s="37"/>
+      <c r="E274" s="49"/>
+      <c r="H274" s="51" t="str">
         <f aca="true">IF(I274 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B275" s="49"/>
-      <c r="C275" s="49"/>
-      <c r="E275" s="50"/>
-      <c r="H275" s="52" t="str">
+      <c r="B275" s="37"/>
+      <c r="C275" s="37"/>
+      <c r="E275" s="49"/>
+      <c r="H275" s="51" t="str">
         <f aca="true">IF(I275 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B276" s="49"/>
-      <c r="C276" s="49"/>
-      <c r="E276" s="50"/>
-      <c r="H276" s="52" t="str">
+      <c r="B276" s="37"/>
+      <c r="C276" s="37"/>
+      <c r="E276" s="49"/>
+      <c r="H276" s="51" t="str">
         <f aca="true">IF(I276 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B277" s="49"/>
-      <c r="C277" s="49"/>
-      <c r="E277" s="50"/>
-      <c r="H277" s="52" t="str">
+      <c r="B277" s="37"/>
+      <c r="C277" s="37"/>
+      <c r="E277" s="49"/>
+      <c r="H277" s="51" t="str">
         <f aca="true">IF(I277 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B278" s="49"/>
-      <c r="C278" s="49"/>
-      <c r="E278" s="50"/>
-      <c r="H278" s="52" t="str">
+      <c r="B278" s="37"/>
+      <c r="C278" s="37"/>
+      <c r="E278" s="49"/>
+      <c r="H278" s="51" t="str">
         <f aca="true">IF(I278 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B279" s="49"/>
-      <c r="C279" s="49"/>
-      <c r="E279" s="50"/>
-      <c r="H279" s="52" t="str">
+      <c r="B279" s="37"/>
+      <c r="C279" s="37"/>
+      <c r="E279" s="49"/>
+      <c r="H279" s="51" t="str">
         <f aca="true">IF(I279 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B280" s="49"/>
-      <c r="C280" s="49"/>
-      <c r="E280" s="50"/>
-      <c r="H280" s="52" t="str">
+      <c r="B280" s="37"/>
+      <c r="C280" s="37"/>
+      <c r="E280" s="49"/>
+      <c r="H280" s="51" t="str">
         <f aca="true">IF(I280 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B281" s="49"/>
-      <c r="C281" s="49"/>
-      <c r="E281" s="50"/>
-      <c r="H281" s="52" t="str">
+      <c r="B281" s="37"/>
+      <c r="C281" s="37"/>
+      <c r="E281" s="49"/>
+      <c r="H281" s="51" t="str">
         <f aca="true">IF(I281 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B282" s="49"/>
-      <c r="C282" s="49"/>
-      <c r="E282" s="50"/>
-      <c r="H282" s="52" t="str">
+      <c r="B282" s="37"/>
+      <c r="C282" s="37"/>
+      <c r="E282" s="49"/>
+      <c r="H282" s="51" t="str">
         <f aca="true">IF(I282 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B283" s="49"/>
-      <c r="C283" s="49"/>
-      <c r="E283" s="50"/>
-      <c r="H283" s="52" t="str">
+      <c r="B283" s="37"/>
+      <c r="C283" s="37"/>
+      <c r="E283" s="49"/>
+      <c r="H283" s="51" t="str">
         <f aca="true">IF(I283 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B284" s="49"/>
-      <c r="C284" s="49"/>
-      <c r="E284" s="50"/>
-      <c r="H284" s="52" t="str">
+      <c r="B284" s="37"/>
+      <c r="C284" s="37"/>
+      <c r="E284" s="49"/>
+      <c r="H284" s="51" t="str">
         <f aca="true">IF(I284 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B285" s="49"/>
-      <c r="C285" s="49"/>
-      <c r="E285" s="50"/>
-      <c r="H285" s="52" t="str">
+      <c r="B285" s="37"/>
+      <c r="C285" s="37"/>
+      <c r="E285" s="49"/>
+      <c r="H285" s="51" t="str">
         <f aca="true">IF(I285 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B286" s="49"/>
-      <c r="C286" s="49"/>
-      <c r="E286" s="50"/>
-      <c r="H286" s="52" t="str">
+      <c r="B286" s="37"/>
+      <c r="C286" s="37"/>
+      <c r="E286" s="49"/>
+      <c r="H286" s="51" t="str">
         <f aca="true">IF(I286 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B287" s="49"/>
-      <c r="C287" s="49"/>
-      <c r="E287" s="50"/>
-      <c r="H287" s="52" t="str">
+      <c r="B287" s="37"/>
+      <c r="C287" s="37"/>
+      <c r="E287" s="49"/>
+      <c r="H287" s="51" t="str">
         <f aca="true">IF(I287 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B288" s="49"/>
-      <c r="C288" s="49"/>
-      <c r="E288" s="50"/>
-      <c r="H288" s="52" t="str">
+      <c r="B288" s="37"/>
+      <c r="C288" s="37"/>
+      <c r="E288" s="49"/>
+      <c r="H288" s="51" t="str">
         <f aca="true">IF(I288 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B289" s="49"/>
-      <c r="C289" s="49"/>
-      <c r="E289" s="50"/>
-      <c r="H289" s="52" t="str">
+      <c r="B289" s="37"/>
+      <c r="C289" s="37"/>
+      <c r="E289" s="49"/>
+      <c r="H289" s="51" t="str">
         <f aca="true">IF(I289 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B290" s="49"/>
-      <c r="C290" s="49"/>
-      <c r="E290" s="50"/>
-      <c r="H290" s="52" t="str">
+      <c r="B290" s="37"/>
+      <c r="C290" s="37"/>
+      <c r="E290" s="49"/>
+      <c r="H290" s="51" t="str">
         <f aca="true">IF(I290 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B291" s="49"/>
-      <c r="C291" s="49"/>
-      <c r="E291" s="50"/>
-      <c r="H291" s="52" t="str">
+      <c r="B291" s="37"/>
+      <c r="C291" s="37"/>
+      <c r="E291" s="49"/>
+      <c r="H291" s="51" t="str">
         <f aca="true">IF(I291 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B292" s="49"/>
-      <c r="C292" s="49"/>
-      <c r="E292" s="50"/>
-      <c r="H292" s="52" t="str">
+      <c r="B292" s="37"/>
+      <c r="C292" s="37"/>
+      <c r="E292" s="49"/>
+      <c r="H292" s="51" t="str">
         <f aca="true">IF(I292 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B293" s="49"/>
-      <c r="C293" s="49"/>
-      <c r="E293" s="50"/>
-      <c r="H293" s="52" t="str">
+      <c r="B293" s="37"/>
+      <c r="C293" s="37"/>
+      <c r="E293" s="49"/>
+      <c r="H293" s="51" t="str">
         <f aca="true">IF(I293 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B294" s="49"/>
-      <c r="C294" s="49"/>
-      <c r="E294" s="50"/>
-      <c r="H294" s="52" t="str">
+      <c r="B294" s="37"/>
+      <c r="C294" s="37"/>
+      <c r="E294" s="49"/>
+      <c r="H294" s="51" t="str">
         <f aca="true">IF(I294 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B295" s="49"/>
-      <c r="C295" s="49"/>
-      <c r="E295" s="50"/>
-      <c r="H295" s="52" t="str">
+      <c r="B295" s="37"/>
+      <c r="C295" s="37"/>
+      <c r="E295" s="49"/>
+      <c r="H295" s="51" t="str">
         <f aca="true">IF(I295 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B296" s="49"/>
-      <c r="C296" s="49"/>
-      <c r="E296" s="50"/>
-      <c r="H296" s="52" t="str">
+      <c r="B296" s="37"/>
+      <c r="C296" s="37"/>
+      <c r="E296" s="49"/>
+      <c r="H296" s="51" t="str">
         <f aca="true">IF(I296 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B297" s="49"/>
-      <c r="C297" s="49"/>
-      <c r="E297" s="50"/>
-      <c r="H297" s="52" t="str">
+      <c r="B297" s="37"/>
+      <c r="C297" s="37"/>
+      <c r="E297" s="49"/>
+      <c r="H297" s="51" t="str">
         <f aca="true">IF(I297 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B298" s="49"/>
-      <c r="C298" s="49"/>
-      <c r="E298" s="50"/>
-      <c r="H298" s="52" t="str">
+      <c r="B298" s="37"/>
+      <c r="C298" s="37"/>
+      <c r="E298" s="49"/>
+      <c r="H298" s="51" t="str">
         <f aca="true">IF(I298 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B299" s="49"/>
-      <c r="C299" s="49"/>
-      <c r="E299" s="50"/>
-      <c r="H299" s="52" t="str">
+      <c r="B299" s="37"/>
+      <c r="C299" s="37"/>
+      <c r="E299" s="49"/>
+      <c r="H299" s="51" t="str">
         <f aca="true">IF(I299 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B300" s="49"/>
-      <c r="C300" s="49"/>
-      <c r="E300" s="50"/>
-      <c r="H300" s="52" t="str">
+      <c r="B300" s="37"/>
+      <c r="C300" s="37"/>
+      <c r="E300" s="49"/>
+      <c r="H300" s="51" t="str">
         <f aca="true">IF(I300 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B301" s="49"/>
-      <c r="C301" s="49"/>
-      <c r="E301" s="50"/>
-      <c r="H301" s="52" t="str">
+      <c r="B301" s="37"/>
+      <c r="C301" s="37"/>
+      <c r="E301" s="49"/>
+      <c r="H301" s="51" t="str">
         <f aca="true">IF(I301 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B302" s="49"/>
-      <c r="C302" s="49"/>
-      <c r="E302" s="50"/>
-      <c r="H302" s="52" t="str">
+      <c r="B302" s="37"/>
+      <c r="C302" s="37"/>
+      <c r="E302" s="49"/>
+      <c r="H302" s="51" t="str">
         <f aca="true">IF(I302 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B303" s="49"/>
-      <c r="C303" s="49"/>
-      <c r="E303" s="50"/>
-      <c r="H303" s="52" t="str">
+      <c r="B303" s="37"/>
+      <c r="C303" s="37"/>
+      <c r="E303" s="49"/>
+      <c r="H303" s="51" t="str">
         <f aca="true">IF(I303 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B304" s="49"/>
-      <c r="C304" s="49"/>
-      <c r="E304" s="50"/>
-      <c r="H304" s="52" t="str">
+      <c r="B304" s="37"/>
+      <c r="C304" s="37"/>
+      <c r="E304" s="49"/>
+      <c r="H304" s="51" t="str">
         <f aca="true">IF(I304 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B305" s="49"/>
-      <c r="C305" s="49"/>
-      <c r="E305" s="50"/>
-      <c r="H305" s="52" t="str">
+      <c r="B305" s="37"/>
+      <c r="C305" s="37"/>
+      <c r="E305" s="49"/>
+      <c r="H305" s="51" t="str">
         <f aca="true">IF(I305 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B306" s="49"/>
-      <c r="C306" s="49"/>
-      <c r="E306" s="50"/>
-      <c r="H306" s="52" t="str">
+      <c r="B306" s="37"/>
+      <c r="C306" s="37"/>
+      <c r="E306" s="49"/>
+      <c r="H306" s="51" t="str">
         <f aca="true">IF(I306 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B307" s="49"/>
-      <c r="C307" s="49"/>
-      <c r="E307" s="50"/>
-      <c r="H307" s="52" t="str">
+      <c r="B307" s="37"/>
+      <c r="C307" s="37"/>
+      <c r="E307" s="49"/>
+      <c r="H307" s="51" t="str">
         <f aca="true">IF(I307 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B308" s="49"/>
-      <c r="C308" s="49"/>
-      <c r="E308" s="50"/>
-      <c r="H308" s="52" t="str">
+      <c r="B308" s="37"/>
+      <c r="C308" s="37"/>
+      <c r="E308" s="49"/>
+      <c r="H308" s="51" t="str">
         <f aca="true">IF(I308 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B309" s="49"/>
-      <c r="C309" s="49"/>
-      <c r="E309" s="50"/>
-      <c r="H309" s="52" t="str">
+      <c r="B309" s="37"/>
+      <c r="C309" s="37"/>
+      <c r="E309" s="49"/>
+      <c r="H309" s="51" t="str">
         <f aca="true">IF(I309 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B310" s="49"/>
-      <c r="C310" s="49"/>
-      <c r="E310" s="50"/>
-      <c r="H310" s="52" t="str">
+      <c r="B310" s="37"/>
+      <c r="C310" s="37"/>
+      <c r="E310" s="49"/>
+      <c r="H310" s="51" t="str">
         <f aca="true">IF(I310 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B311" s="49"/>
-      <c r="C311" s="49"/>
-      <c r="E311" s="50"/>
-      <c r="H311" s="52" t="str">
+      <c r="B311" s="37"/>
+      <c r="C311" s="37"/>
+      <c r="E311" s="49"/>
+      <c r="H311" s="51" t="str">
         <f aca="true">IF(I311 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B312" s="49"/>
-      <c r="C312" s="49"/>
-      <c r="E312" s="50"/>
-      <c r="H312" s="52" t="str">
+      <c r="B312" s="37"/>
+      <c r="C312" s="37"/>
+      <c r="E312" s="49"/>
+      <c r="H312" s="51" t="str">
         <f aca="true">IF(I312 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B313" s="49"/>
-      <c r="C313" s="49"/>
-      <c r="E313" s="50"/>
-      <c r="H313" s="52" t="str">
+      <c r="B313" s="37"/>
+      <c r="C313" s="37"/>
+      <c r="E313" s="49"/>
+      <c r="H313" s="51" t="str">
         <f aca="true">IF(I313 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B314" s="49"/>
-      <c r="C314" s="49"/>
-      <c r="E314" s="50"/>
-      <c r="H314" s="52" t="str">
+      <c r="B314" s="37"/>
+      <c r="C314" s="37"/>
+      <c r="E314" s="49"/>
+      <c r="H314" s="51" t="str">
         <f aca="true">IF(I314 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B315" s="49"/>
-      <c r="C315" s="49"/>
-      <c r="E315" s="50"/>
-      <c r="H315" s="52" t="str">
+      <c r="B315" s="37"/>
+      <c r="C315" s="37"/>
+      <c r="E315" s="49"/>
+      <c r="H315" s="51" t="str">
         <f aca="true">IF(I315 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B316" s="49"/>
-      <c r="C316" s="49"/>
-      <c r="E316" s="50"/>
-      <c r="H316" s="52" t="str">
+      <c r="B316" s="37"/>
+      <c r="C316" s="37"/>
+      <c r="E316" s="49"/>
+      <c r="H316" s="51" t="str">
         <f aca="true">IF(I316 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B317" s="49"/>
-      <c r="C317" s="49"/>
-      <c r="E317" s="50"/>
-      <c r="H317" s="52" t="str">
+      <c r="B317" s="37"/>
+      <c r="C317" s="37"/>
+      <c r="E317" s="49"/>
+      <c r="H317" s="51" t="str">
         <f aca="true">IF(I317 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B318" s="49"/>
-      <c r="C318" s="49"/>
-      <c r="E318" s="50"/>
-      <c r="H318" s="52" t="str">
+      <c r="B318" s="37"/>
+      <c r="C318" s="37"/>
+      <c r="E318" s="49"/>
+      <c r="H318" s="51" t="str">
         <f aca="true">IF(I318 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B319" s="49"/>
-      <c r="C319" s="49"/>
-      <c r="E319" s="50"/>
-      <c r="H319" s="52" t="str">
+      <c r="B319" s="37"/>
+      <c r="C319" s="37"/>
+      <c r="E319" s="49"/>
+      <c r="H319" s="51" t="str">
         <f aca="true">IF(I319 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B320" s="49"/>
-      <c r="C320" s="49"/>
-      <c r="H320" s="52" t="str">
+      <c r="B320" s="37"/>
+      <c r="C320" s="37"/>
+      <c r="H320" s="51" t="str">
         <f aca="true">IF(I320 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B321" s="49"/>
-      <c r="C321" s="49"/>
-      <c r="H321" s="52" t="str">
+      <c r="B321" s="37"/>
+      <c r="C321" s="37"/>
+      <c r="H321" s="51" t="str">
         <f aca="true">IF(I321 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B322" s="49"/>
-      <c r="C322" s="49"/>
-      <c r="H322" s="52" t="str">
+      <c r="B322" s="37"/>
+      <c r="C322" s="37"/>
+      <c r="H322" s="51" t="str">
         <f aca="true">IF(I322 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B323" s="49"/>
-      <c r="C323" s="49"/>
-      <c r="H323" s="52" t="str">
+      <c r="B323" s="37"/>
+      <c r="C323" s="37"/>
+      <c r="H323" s="51" t="str">
         <f aca="true">IF(I323 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B324" s="49"/>
-      <c r="C324" s="49"/>
-      <c r="H324" s="52" t="str">
+      <c r="B324" s="37"/>
+      <c r="C324" s="37"/>
+      <c r="H324" s="51" t="str">
         <f aca="true">IF(I324 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B325" s="49"/>
-      <c r="C325" s="49"/>
+      <c r="B325" s="37"/>
+      <c r="C325" s="37"/>
     </row>
     <row r="326" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B326" s="49"/>
-      <c r="C326" s="49"/>
+      <c r="B326" s="37"/>
+      <c r="C326" s="37"/>
     </row>
     <row r="327" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B327" s="49"/>
-      <c r="C327" s="49"/>
+      <c r="B327" s="37"/>
+      <c r="C327" s="37"/>
     </row>
     <row r="328" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B328" s="49"/>
-      <c r="C328" s="49"/>
+      <c r="B328" s="37"/>
+      <c r="C328" s="37"/>
     </row>
     <row r="329" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B329" s="49"/>
-      <c r="C329" s="49"/>
+      <c r="B329" s="37"/>
+      <c r="C329" s="37"/>
     </row>
     <row r="330" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B330" s="49"/>
-      <c r="C330" s="49"/>
+      <c r="B330" s="37"/>
+      <c r="C330" s="37"/>
     </row>
     <row r="331" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B331" s="49"/>
-      <c r="C331" s="49"/>
+      <c r="B331" s="37"/>
+      <c r="C331" s="37"/>
     </row>
     <row r="332" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B332" s="49"/>
-      <c r="C332" s="49"/>
+      <c r="B332" s="37"/>
+      <c r="C332" s="37"/>
     </row>
     <row r="333" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B333" s="49"/>
-      <c r="C333" s="49"/>
+      <c r="B333" s="37"/>
+      <c r="C333" s="37"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -17751,36 +17747,36 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="55" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54" t="s">
+    <row r="1" s="54" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="53"/>
+      <c r="B1" s="53" t="s">
         <v>424</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="53" t="s">
         <v>425</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="53" t="s">
         <v>426</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="53" t="s">
         <v>427</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="53" t="s">
         <v>428</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="53" t="s">
         <v>429</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="53" t="s">
         <v>430</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="53" t="s">
         <v>431</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="53" t="s">
         <v>432</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="53" t="s">
         <v>411</v>
       </c>
     </row>

</xml_diff>